<commit_message>
EUR, USD, GBP LCH
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR/EUR_YCSTDBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR/EUR_YCSTDBootstrapping.xlsx
@@ -1680,7 +1680,9 @@
       <c r="C5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="21"/>
+      <c r="D5" s="21">
+        <v>42306.799166666664</v>
+      </c>
       <c r="E5" s="80"/>
     </row>
     <row r="6" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1747,7 +1749,7 @@
       </c>
       <c r="D12" s="13">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>42270</v>
+        <v>42304</v>
       </c>
       <c r="E12" s="80"/>
     </row>
@@ -1758,7 +1760,7 @@
       </c>
       <c r="D13" s="15">
         <f>_xll.qlCalendarAdvance(Calendar,Evaluationdate,"2D","F",,Trigger)</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="E13" s="80"/>
     </row>
@@ -1790,8 +1792,8 @@
         <v>10</v>
       </c>
       <c r="D18" s="41" t="str">
-        <f>_xll.qlPiecewiseYieldCurve(D20,D21,Calendar,_xll.ohPack(RateHelpersSTD),,,,D22,D23,D24,Permanent,,ObjectOverwrite)</f>
-        <v>_EURSTD#0002</v>
+        <f>_xll.qlPiecewiseYieldCurve(D20,D21,Calendar,_xll.ohPack(RateHelpersSTD),,,,D22,D23,D24,,Permanent,,ObjectOverwrite)</f>
+        <v>_EURSTD#0001</v>
       </c>
       <c r="E18" s="42"/>
     </row>
@@ -1869,7 +1871,7 @@
       <c r="B26" s="23"/>
       <c r="C26" s="32">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve_STD)</f>
-        <v>42270</v>
+        <v>42304</v>
       </c>
       <c r="D26" s="33">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C26,,Trigger)</f>
@@ -1882,11 +1884,11 @@
       <c r="B27" s="23"/>
       <c r="C27" s="34">
         <f>_xll.qlTermStructureMaxDate(YieldCurve_STD,Trigger)</f>
-        <v>64194</v>
+        <v>64221</v>
       </c>
       <c r="D27" s="35">
         <f>_xll.qlYieldTSDiscount(YieldCurve_STD,C27,,Trigger)</f>
-        <v>0.40831451668537344</v>
+        <v>0.43450268875829101</v>
       </c>
       <c r="E27" s="42"/>
     </row>
@@ -1956,7 +1958,7 @@
   <dimension ref="A1:AH127"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2100,7 +2102,7 @@
       </c>
       <c r="AC2" s="155">
         <f t="array" ref="AC2:AC89">_xll.qlPiecewiseYieldCurveData(YieldCurve_STD,Trigger)</f>
-        <v>-1.318057935357494E-3</v>
+        <v>-1.2166686944639845E-3</v>
       </c>
       <c r="AE2" s="160" t="s">
         <v>73</v>
@@ -2131,7 +2133,7 @@
       <c r="I3" s="120"/>
       <c r="J3" s="110" t="str">
         <f>_xll.qlDepositRateHelper(,H3,G3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00575#0001</v>
+        <v>obj_0057a#0000</v>
       </c>
       <c r="K3" s="49"/>
       <c r="L3" s="66" t="str">
@@ -2140,7 +2142,7 @@
       </c>
       <c r="M3" s="128" t="str">
         <f>IF(ISBLANK(J3),"--",J3)</f>
-        <v>obj_00575#0001</v>
+        <v>obj_0057a#0000</v>
       </c>
       <c r="N3" s="142" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M3,Trigger),"--")</f>
@@ -2148,7 +2150,7 @@
       </c>
       <c r="O3" s="130">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M3,Trigger),"--")</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="P3" s="129" t="b">
         <v>1</v>
@@ -2161,11 +2163,11 @@
       </c>
       <c r="S3" s="131">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M3,Trigger),"--")</f>
-        <v>42270</v>
+        <v>42304</v>
       </c>
       <c r="T3" s="131">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M3,Trigger),"--")</f>
-        <v>42271</v>
+        <v>42305</v>
       </c>
       <c r="U3" s="159"/>
       <c r="V3" s="3" t="str">
@@ -2174,7 +2176,7 @@
       </c>
       <c r="W3" s="3" t="str">
         <f t="array" ref="W3:W89">_xll.qlRateHelperSelection(_xll.ohFilter(RateHelpers,IncludeFlag),_xll.ohFilter(Priority,IncludeFlag),$AF$3,$AF$4,$AF$5,$AF$6,_xll.ohFilter(MinDistance,IncludeFlag),Trigger)</f>
-        <v>obj_00575</v>
+        <v>obj_0057a</v>
       </c>
       <c r="X3" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W3,Trigger),"")</f>
@@ -2182,7 +2184,7 @@
       </c>
       <c r="Y3" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W3,Trigger),"")</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="Z3" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W3)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W3)),_xll.qlSwapRateHelperSpread($W3))</f>
@@ -2190,14 +2192,14 @@
       </c>
       <c r="AA3" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W3,Trigger),"")</f>
-        <v>42270</v>
+        <v>42304</v>
       </c>
       <c r="AB3" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W3,Trigger),"")</f>
-        <v>42271</v>
+        <v>42305</v>
       </c>
       <c r="AC3" s="68">
-        <v>-1.318057935357494E-3</v>
+        <v>-1.2166686944639845E-3</v>
       </c>
       <c r="AD3" s="158"/>
       <c r="AE3" s="103" t="s">
@@ -2231,7 +2233,7 @@
       <c r="I4" s="127"/>
       <c r="J4" s="57" t="str">
         <f>_xll.qlFraRateHelper(,H4,"1D",G4,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00566#0001</v>
+        <v>obj_0055a#0000</v>
       </c>
       <c r="K4" s="48"/>
       <c r="L4" s="9" t="str">
@@ -2240,7 +2242,7 @@
       </c>
       <c r="M4" s="90" t="str">
         <f t="shared" ref="M4:M11" si="3">IF(ISBLANK(J4),"--",J4)</f>
-        <v>obj_00566#0001</v>
+        <v>obj_0055a#0000</v>
       </c>
       <c r="N4" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M4,Trigger),"--")</f>
@@ -2248,7 +2250,7 @@
       </c>
       <c r="O4" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M4,Trigger),"--")</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="P4" s="93" t="b">
         <v>1</v>
@@ -2261,11 +2263,11 @@
       </c>
       <c r="S4" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M4,Trigger),"--")</f>
-        <v>42271</v>
+        <v>42305</v>
       </c>
       <c r="T4" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M4,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="U4" s="159"/>
       <c r="V4" s="3" t="str">
@@ -2273,7 +2275,7 @@
         <v>Dp</v>
       </c>
       <c r="W4" s="3" t="str">
-        <v>obj_00566</v>
+        <v>obj_0055a</v>
       </c>
       <c r="X4" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W4,Trigger),"")</f>
@@ -2281,7 +2283,7 @@
       </c>
       <c r="Y4" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W4,Trigger),"")</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="Z4" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W4)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W4)),_xll.qlSwapRateHelperSpread($W4))</f>
@@ -2289,14 +2291,14 @@
       </c>
       <c r="AA4" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W4,Trigger),"")</f>
-        <v>42271</v>
+        <v>42305</v>
       </c>
       <c r="AB4" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W4,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AC4" s="68">
-        <v>-1.3180579353314684E-3</v>
+        <v>-1.2166686944770151E-3</v>
       </c>
       <c r="AD4" s="158"/>
       <c r="AE4" s="103" t="s">
@@ -2330,7 +2332,7 @@
       <c r="I5" s="122"/>
       <c r="J5" s="2" t="str">
         <f>_xll.qlFraRateHelper(,H5,"2D",G5,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00574#0001</v>
+        <v>obj_0057d#0000</v>
       </c>
       <c r="K5" s="48"/>
       <c r="L5" s="9" t="str">
@@ -2339,7 +2341,7 @@
       </c>
       <c r="M5" s="90" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00574#0001</v>
+        <v>obj_0057d#0000</v>
       </c>
       <c r="N5" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M5,Trigger),"--")</f>
@@ -2347,7 +2349,7 @@
       </c>
       <c r="O5" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M5,Trigger),"--")</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="P5" s="93" t="b">
         <v>1</v>
@@ -2360,11 +2362,11 @@
       </c>
       <c r="S5" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M5,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T5" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M5,Trigger),"--")</f>
-        <v>42275</v>
+        <v>42307</v>
       </c>
       <c r="U5" s="159"/>
       <c r="V5" s="3" t="str">
@@ -2372,7 +2374,7 @@
         <v>Dp</v>
       </c>
       <c r="W5" s="3" t="str">
-        <v>obj_00574</v>
+        <v>obj_0057d</v>
       </c>
       <c r="X5" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W5,Trigger),"")</f>
@@ -2380,7 +2382,7 @@
       </c>
       <c r="Y5" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W5,Trigger),"")</f>
-        <v>-1.2999999999999999E-3</v>
+        <v>-1.1999999999999999E-3</v>
       </c>
       <c r="Z5" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W5)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W5)),_xll.qlSwapRateHelperSpread($W5))</f>
@@ -2388,14 +2390,14 @@
       </c>
       <c r="AA5" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W5,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB5" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W5,Trigger),"")</f>
-        <v>42275</v>
+        <v>42307</v>
       </c>
       <c r="AC5" s="68">
-        <v>-1.318060791188344E-3</v>
+        <v>-1.2166686944926031E-3</v>
       </c>
       <c r="AD5" s="158"/>
       <c r="AE5" s="103" t="s">
@@ -2431,7 +2433,7 @@
       <c r="I6" s="121"/>
       <c r="J6" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H6,G6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00576#0001</v>
+        <v>obj_0057b#0000</v>
       </c>
       <c r="K6" s="48"/>
       <c r="L6" s="9" t="str">
@@ -2440,7 +2442,7 @@
       </c>
       <c r="M6" s="90" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00576#0001</v>
+        <v>obj_0057b#0000</v>
       </c>
       <c r="N6" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M6,Trigger),"--")</f>
@@ -2448,7 +2450,7 @@
       </c>
       <c r="O6" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M6,Trigger),"--")</f>
-        <v>-1.4099999999999998E-3</v>
+        <v>-1.47E-3</v>
       </c>
       <c r="P6" s="93" t="b">
         <v>1</v>
@@ -2461,11 +2463,11 @@
       </c>
       <c r="S6" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M6,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T6" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M6,Trigger),"--")</f>
-        <v>42279</v>
+        <v>42313</v>
       </c>
       <c r="U6" s="159"/>
       <c r="V6" s="3" t="str">
@@ -2473,7 +2475,7 @@
         <v>Dp</v>
       </c>
       <c r="W6" s="3" t="str">
-        <v>obj_00576</v>
+        <v>obj_0057b</v>
       </c>
       <c r="X6" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W6,Trigger),"")</f>
@@ -2481,7 +2483,7 @@
       </c>
       <c r="Y6" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W6,Trigger),"")</f>
-        <v>-1.4099999999999998E-3</v>
+        <v>-1.47E-3</v>
       </c>
       <c r="Z6" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W6)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W6)),_xll.qlSwapRateHelperSpread($W6))</f>
@@ -2489,14 +2491,14 @@
       </c>
       <c r="AA6" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W6,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB6" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W6,Trigger),"")</f>
-        <v>42279</v>
+        <v>42313</v>
       </c>
       <c r="AC6" s="68">
-        <v>-1.4048151541028934E-3</v>
+        <v>-1.4296003513532606E-3</v>
       </c>
       <c r="AD6" s="158"/>
       <c r="AE6" s="103" t="s">
@@ -2532,7 +2534,7 @@
       <c r="I7" s="121"/>
       <c r="J7" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H7,G7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00573#0001</v>
+        <v>obj_00579#0000</v>
       </c>
       <c r="K7" s="48"/>
       <c r="L7" s="9" t="str">
@@ -2541,7 +2543,7 @@
       </c>
       <c r="M7" s="90" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00573#0001</v>
+        <v>obj_00579#0000</v>
       </c>
       <c r="N7" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M7,Trigger),"--")</f>
@@ -2549,7 +2551,7 @@
       </c>
       <c r="O7" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M7,Trigger),"--")</f>
-        <v>-1.0700000000000002E-3</v>
+        <v>-1.1899999999999999E-3</v>
       </c>
       <c r="P7" s="93" t="b">
         <v>1</v>
@@ -2562,11 +2564,11 @@
       </c>
       <c r="S7" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M7,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T7" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M7,Trigger),"--")</f>
-        <v>42303</v>
+        <v>42338</v>
       </c>
       <c r="U7" s="159"/>
       <c r="V7" s="3" t="str">
@@ -2574,7 +2576,7 @@
         <v>Dp</v>
       </c>
       <c r="W7" s="3" t="str">
-        <v>obj_00573</v>
+        <v>obj_00579</v>
       </c>
       <c r="X7" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W7,Trigger),"")</f>
@@ -2582,7 +2584,7 @@
       </c>
       <c r="Y7" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W7,Trigger),"")</f>
-        <v>-1.0700000000000002E-3</v>
+        <v>-1.1899999999999999E-3</v>
       </c>
       <c r="Z7" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W7)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W7)),_xll.qlSwapRateHelperSpread($W7))</f>
@@ -2590,14 +2592,14 @@
       </c>
       <c r="AA7" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W7,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB7" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W7,Trigger),"")</f>
-        <v>42303</v>
+        <v>42338</v>
       </c>
       <c r="AC7" s="68">
-        <v>-1.0990412047792346E-3</v>
+        <v>-1.2071843647970045E-3</v>
       </c>
       <c r="AD7" s="158"/>
       <c r="AH7" s="156"/>
@@ -2627,7 +2629,7 @@
       <c r="I8" s="121"/>
       <c r="J8" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H8,G8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00572#0001</v>
+        <v>obj_0057c#0000</v>
       </c>
       <c r="K8" s="48"/>
       <c r="L8" s="9" t="str">
@@ -2636,7 +2638,7 @@
       </c>
       <c r="M8" s="90" t="str">
         <f t="shared" si="3"/>
-        <v>obj_00572#0001</v>
+        <v>obj_0057c#0000</v>
       </c>
       <c r="N8" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M8,Trigger),"--")</f>
@@ -2644,7 +2646,7 @@
       </c>
       <c r="O8" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M8,Trigger),"--")</f>
-        <v>-6.5999999999999989E-4</v>
+        <v>-8.4000000000000003E-4</v>
       </c>
       <c r="P8" s="93" t="b">
         <v>1</v>
@@ -2657,11 +2659,11 @@
       </c>
       <c r="S8" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M8,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T8" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M8,Trigger),"--")</f>
-        <v>42333</v>
+        <v>42367</v>
       </c>
       <c r="U8" s="159"/>
       <c r="V8" s="3" t="str">
@@ -2669,7 +2671,7 @@
         <v>Dp</v>
       </c>
       <c r="W8" s="3" t="str">
-        <v>obj_00572</v>
+        <v>obj_0057c</v>
       </c>
       <c r="X8" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W8,Trigger),"")</f>
@@ -2677,7 +2679,7 @@
       </c>
       <c r="Y8" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W8,Trigger),"")</f>
-        <v>-6.5999999999999989E-4</v>
+        <v>-8.4000000000000003E-4</v>
       </c>
       <c r="Z8" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W8)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W8)),_xll.qlSwapRateHelperSpread($W8))</f>
@@ -2685,14 +2687,14 @@
       </c>
       <c r="AA8" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W8,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB8" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W8,Trigger),"")</f>
-        <v>42333</v>
+        <v>42367</v>
       </c>
       <c r="AC8" s="68">
-        <v>-6.8980262189384013E-4</v>
+        <v>-8.633127243400314E-4</v>
       </c>
       <c r="AD8" s="158"/>
       <c r="AH8" s="156"/>
@@ -2722,7 +2724,7 @@
       <c r="I9" s="121"/>
       <c r="J9" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H9,G9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0054f#0001</v>
+        <v>obj_00556#0000</v>
       </c>
       <c r="K9" s="48"/>
       <c r="L9" s="9" t="str">
@@ -2731,7 +2733,7 @@
       </c>
       <c r="M9" s="90" t="str">
         <f t="shared" si="3"/>
-        <v>obj_0054f#0001</v>
+        <v>obj_00556#0000</v>
       </c>
       <c r="N9" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M9,Trigger),"--")</f>
@@ -2739,7 +2741,7 @@
       </c>
       <c r="O9" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M9,Trigger),"--")</f>
-        <v>-3.8999999999999999E-4</v>
+        <v>-6.5999999999999989E-4</v>
       </c>
       <c r="P9" s="93" t="b">
         <v>1</v>
@@ -2752,11 +2754,11 @@
       </c>
       <c r="S9" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M9,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T9" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M9,Trigger),"--")</f>
-        <v>42366</v>
+        <v>42398</v>
       </c>
       <c r="U9" s="159"/>
       <c r="V9" s="3" t="str">
@@ -2764,7 +2766,7 @@
         <v>Dp</v>
       </c>
       <c r="W9" s="3" t="str">
-        <v>obj_0054f</v>
+        <v>obj_00556</v>
       </c>
       <c r="X9" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W9,Trigger),"")</f>
@@ -2772,7 +2774,7 @@
       </c>
       <c r="Y9" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W9,Trigger),"")</f>
-        <v>-3.8999999999999999E-4</v>
+        <v>-6.5999999999999989E-4</v>
       </c>
       <c r="Z9" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W9)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W9)),_xll.qlSwapRateHelperSpread($W9))</f>
@@ -2780,14 +2782,14 @@
       </c>
       <c r="AA9" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W9,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB9" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W9,Trigger),"")</f>
-        <v>42366</v>
+        <v>42398</v>
       </c>
       <c r="AC9" s="68">
-        <v>-4.1465807495714882E-4</v>
+        <v>-6.8087088454500168E-4</v>
       </c>
       <c r="AD9" s="158"/>
       <c r="AH9" s="156"/>
@@ -2817,7 +2819,7 @@
       <c r="I10" s="121"/>
       <c r="J10" s="62" t="str">
         <f>_xll.qlDepositRateHelper(,H10,G10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0054e#0001</v>
+        <v>obj_00555#0000</v>
       </c>
       <c r="K10" s="48" t="s">
         <v>36</v>
@@ -2828,7 +2830,7 @@
       </c>
       <c r="M10" s="90" t="str">
         <f t="shared" si="3"/>
-        <v>obj_0054e#0001</v>
+        <v>obj_00555#0000</v>
       </c>
       <c r="N10" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M10,Trigger),"--")</f>
@@ -2836,7 +2838,7 @@
       </c>
       <c r="O10" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M10,Trigger),"--")</f>
-        <v>3.2999999999999994E-4</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="P10" s="93" t="b">
         <v>1</v>
@@ -2849,11 +2851,11 @@
       </c>
       <c r="S10" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M10,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T10" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M10,Trigger),"--")</f>
-        <v>42458</v>
+        <v>42489</v>
       </c>
       <c r="U10" s="159"/>
       <c r="V10" s="3" t="str">
@@ -2861,7 +2863,7 @@
         <v>Dp</v>
       </c>
       <c r="W10" s="3" t="str">
-        <v>obj_0054e</v>
+        <v>obj_00555</v>
       </c>
       <c r="X10" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W10,Trigger),"")</f>
@@ -2869,7 +2871,7 @@
       </c>
       <c r="Y10" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W10,Trigger),"")</f>
-        <v>3.2999999999999994E-4</v>
+        <v>8.0000000000000007E-5</v>
       </c>
       <c r="Z10" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W10)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W10)),_xll.qlSwapRateHelperSpread($W10))</f>
@@ -2877,14 +2879,14 @@
       </c>
       <c r="AA10" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W10,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB10" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W10,Trigger),"")</f>
-        <v>42458</v>
+        <v>42489</v>
       </c>
       <c r="AC10" s="68">
-        <v>3.1697382665782522E-4</v>
+        <v>6.707942776379395E-5</v>
       </c>
       <c r="AD10" s="158"/>
       <c r="AH10" s="156"/>
@@ -2953,7 +2955,7 @@
         <v>FRA</v>
       </c>
       <c r="W11" s="3" t="str">
-        <v>obj_0054c</v>
+        <v>obj_0054e</v>
       </c>
       <c r="X11" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W11,Trigger),"")</f>
@@ -2961,7 +2963,7 @@
       </c>
       <c r="Y11" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W11,Trigger),"")</f>
-        <v>2.5000000000000001E-4</v>
+        <v>-7.8000000000000009E-4</v>
       </c>
       <c r="Z11" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W11)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W11)),_xll.qlSwapRateHelperSpread($W11))</f>
@@ -2969,14 +2971,14 @@
       </c>
       <c r="AA11" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W11,Trigger),"")</f>
-        <v>42458</v>
+        <v>42489</v>
       </c>
       <c r="AB11" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W11,Trigger),"")</f>
-        <v>42639</v>
+        <v>42674</v>
       </c>
       <c r="AC11" s="68">
-        <v>2.845272062160261E-4</v>
+        <v>-3.6195622205835844E-4</v>
       </c>
       <c r="AD11" s="158"/>
       <c r="AH11" s="156"/>
@@ -3030,7 +3032,7 @@
         <v>FRA</v>
       </c>
       <c r="W12" s="3" t="str">
-        <v>obj_0054b</v>
+        <v>obj_00552</v>
       </c>
       <c r="X12" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W12,Trigger),"")</f>
@@ -3038,7 +3040,7 @@
       </c>
       <c r="Y12" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W12,Trigger),"")</f>
-        <v>2.7000000000000006E-4</v>
+        <v>-8.200000000000002E-4</v>
       </c>
       <c r="Z12" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W12)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W12)),_xll.qlSwapRateHelperSpread($W12))</f>
@@ -3046,14 +3048,14 @@
       </c>
       <c r="AA12" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W12,Trigger),"")</f>
-        <v>42485</v>
+        <v>42520</v>
       </c>
       <c r="AB12" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W12,Trigger),"")</f>
-        <v>42668</v>
+        <v>42703</v>
       </c>
       <c r="AC12" s="68">
-        <v>2.9447628859980655E-4</v>
+        <v>-3.8439695338718881E-4</v>
       </c>
       <c r="AD12" s="158"/>
       <c r="AH12" s="156"/>
@@ -3120,7 +3122,7 @@
         <v>FRA</v>
       </c>
       <c r="W13" s="3" t="str">
-        <v>obj_0054a</v>
+        <v>obj_0054f</v>
       </c>
       <c r="X13" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W13,Trigger),"")</f>
@@ -3128,7 +3130,7 @@
       </c>
       <c r="Y13" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W13,Trigger),"")</f>
-        <v>2.8000000000000003E-4</v>
+        <v>-8.4000000000000014E-4</v>
       </c>
       <c r="Z13" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W13)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W13)),_xll.qlSwapRateHelperSpread($W13))</f>
@@ -3136,14 +3138,14 @@
       </c>
       <c r="AA13" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W13,Trigger),"")</f>
-        <v>42515</v>
+        <v>42550</v>
       </c>
       <c r="AB13" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W13,Trigger),"")</f>
-        <v>42699</v>
+        <v>42733</v>
       </c>
       <c r="AC13" s="68">
-        <v>2.9693938561244022E-4</v>
+        <v>-4.0603108235821048E-4</v>
       </c>
       <c r="AD13" s="158"/>
       <c r="AH13" s="156"/>
@@ -3211,7 +3213,7 @@
         <v>FRA</v>
       </c>
       <c r="W14" s="3" t="str">
-        <v>obj_00546</v>
+        <v>obj_00551</v>
       </c>
       <c r="X14" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W14,Trigger),"")</f>
@@ -3219,7 +3221,7 @@
       </c>
       <c r="Y14" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W14,Trigger),"")</f>
-        <v>3.0999999999999995E-4</v>
+        <v>-8.3000000000000001E-4</v>
       </c>
       <c r="Z14" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W14)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W14)),_xll.qlSwapRateHelperSpread($W14))</f>
@@ -3227,14 +3229,14 @@
       </c>
       <c r="AA14" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W14,Trigger),"")</f>
-        <v>42548</v>
+        <v>42580</v>
       </c>
       <c r="AB14" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W14,Trigger),"")</f>
-        <v>42731</v>
+        <v>42765</v>
       </c>
       <c r="AC14" s="68">
-        <v>3.0617558809858079E-4</v>
+        <v>-4.2398870312483725E-4</v>
       </c>
       <c r="AD14" s="158"/>
       <c r="AH14" s="156"/>
@@ -3302,7 +3304,7 @@
         <v>FRA</v>
       </c>
       <c r="W15" s="3" t="str">
-        <v>obj_0054d</v>
+        <v>obj_00550</v>
       </c>
       <c r="X15" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W15,Trigger),"")</f>
@@ -3310,7 +3312,7 @@
       </c>
       <c r="Y15" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W15,Trigger),"")</f>
-        <v>3.5999999999999997E-4</v>
+        <v>-8.3000000000000001E-4</v>
       </c>
       <c r="Z15" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W15)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W15)),_xll.qlSwapRateHelperSpread($W15))</f>
@@ -3318,14 +3320,14 @@
       </c>
       <c r="AA15" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W15,Trigger),"")</f>
-        <v>42576</v>
+        <v>42611</v>
       </c>
       <c r="AB15" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W15,Trigger),"")</f>
-        <v>42760</v>
+        <v>42794</v>
       </c>
       <c r="AC15" s="68">
-        <v>3.2178567503361147E-4</v>
+        <v>-4.4958918833965753E-4</v>
       </c>
       <c r="AD15" s="158"/>
       <c r="AH15" s="156"/>
@@ -3393,7 +3395,7 @@
         <v>FRA</v>
       </c>
       <c r="W16" s="3" t="str">
-        <v>obj_00549</v>
+        <v>obj_00554</v>
       </c>
       <c r="X16" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W16,Trigger),"")</f>
@@ -3401,7 +3403,7 @@
       </c>
       <c r="Y16" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W16,Trigger),"")</f>
-        <v>4.0999999999999994E-4</v>
+        <v>-8.0000000000000015E-4</v>
       </c>
       <c r="Z16" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W16)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W16)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W16)),_xll.qlSwapRateHelperSpread($W16))</f>
@@ -3409,14 +3411,14 @@
       </c>
       <c r="AA16" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W16,Trigger),"")</f>
-        <v>42607</v>
+        <v>42642</v>
       </c>
       <c r="AB16" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W16,Trigger),"")</f>
-        <v>42793</v>
+        <v>42823</v>
       </c>
       <c r="AC16" s="68">
-        <v>3.3485625176862805E-4</v>
+        <v>-4.7032434709642966E-4</v>
       </c>
       <c r="AD16" s="158"/>
       <c r="AH16" s="156"/>
@@ -3452,7 +3454,7 @@
       </c>
       <c r="M17" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_0054c#0001</v>
+        <v>obj_0054e#0000</v>
       </c>
       <c r="N17" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M17,Trigger),"--")</f>
@@ -3460,7 +3462,7 @@
       </c>
       <c r="O17" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M17,Trigger),"--")</f>
-        <v>2.5000000000000001E-4</v>
+        <v>-7.8000000000000009E-4</v>
       </c>
       <c r="P17" s="93" t="b">
         <v>1</v>
@@ -3473,18 +3475,18 @@
       </c>
       <c r="S17" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M17,Trigger),"--")</f>
-        <v>42458</v>
+        <v>42489</v>
       </c>
       <c r="T17" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M17,Trigger),"--")</f>
-        <v>42639</v>
+        <v>42674</v>
       </c>
       <c r="V17" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FRA</v>
       </c>
       <c r="W17" s="3" t="str">
-        <v>obj_00547</v>
+        <v>obj_00553</v>
       </c>
       <c r="X17" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W17,Trigger),"")</f>
@@ -3492,7 +3494,7 @@
       </c>
       <c r="Y17" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W17,Trigger),"")</f>
-        <v>4.6999999999999999E-4</v>
+        <v>-7.400000000000001E-4</v>
       </c>
       <c r="Z17" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W17)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W17)),_xll.qlSwapRateHelperSpread($W17))</f>
@@ -3500,14 +3502,14 @@
       </c>
       <c r="AA17" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W17,Trigger),"")</f>
-        <v>42639</v>
+        <v>42674</v>
       </c>
       <c r="AB17" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W17,Trigger),"")</f>
-        <v>42821</v>
+        <v>42853</v>
       </c>
       <c r="AC17" s="68">
-        <v>3.4792793558608895E-4</v>
+        <v>-4.8861245512661438E-4</v>
       </c>
       <c r="AD17" s="158"/>
       <c r="AH17" s="156"/>
@@ -3543,7 +3545,7 @@
       </c>
       <c r="M18" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_0054b#0001</v>
+        <v>obj_00552#0000</v>
       </c>
       <c r="N18" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M18,Trigger),"--")</f>
@@ -3551,7 +3553,7 @@
       </c>
       <c r="O18" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M18,Trigger),"--")</f>
-        <v>2.7000000000000006E-4</v>
+        <v>-8.200000000000002E-4</v>
       </c>
       <c r="P18" s="93" t="b">
         <v>1</v>
@@ -3564,18 +3566,18 @@
       </c>
       <c r="S18" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M18,Trigger),"--")</f>
-        <v>42485</v>
+        <v>42520</v>
       </c>
       <c r="T18" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M18,Trigger),"--")</f>
-        <v>42668</v>
+        <v>42703</v>
       </c>
       <c r="V18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>FRA</v>
       </c>
       <c r="W18" s="3" t="str">
-        <v>obj_00548</v>
+        <v>obj_0054d</v>
       </c>
       <c r="X18" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W18,Trigger),"")</f>
@@ -3583,7 +3585,7 @@
       </c>
       <c r="Y18" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W18,Trigger),"")</f>
-        <v>7.6000000000000015E-4</v>
+        <v>-5.2999999999999998E-4</v>
       </c>
       <c r="Z18" s="100" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W18)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W18)),_xll.qlSwapRateHelperSpread($W18))</f>
@@ -3591,14 +3593,14 @@
       </c>
       <c r="AA18" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W18,Trigger),"")</f>
-        <v>42731</v>
+        <v>42765</v>
       </c>
       <c r="AB18" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W18,Trigger),"")</f>
-        <v>42912</v>
+        <v>42947</v>
       </c>
       <c r="AC18" s="68">
-        <v>4.3617103811774817E-4</v>
+        <v>-4.5609894113512561E-4</v>
       </c>
       <c r="AD18" s="158"/>
       <c r="AH18" s="156"/>
@@ -3628,7 +3630,7 @@
       <c r="I19" s="121"/>
       <c r="J19" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H19,B19&amp;"M",G19,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0054c#0001</v>
+        <v>obj_0054e#0000</v>
       </c>
       <c r="K19" s="48"/>
       <c r="L19" s="9" t="str">
@@ -3637,7 +3639,7 @@
       </c>
       <c r="M19" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_0054a#0001</v>
+        <v>obj_0054f#0000</v>
       </c>
       <c r="N19" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M19,Trigger),"--")</f>
@@ -3645,7 +3647,7 @@
       </c>
       <c r="O19" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M19,Trigger),"--")</f>
-        <v>2.8000000000000003E-4</v>
+        <v>-8.4000000000000014E-4</v>
       </c>
       <c r="P19" s="93" t="b">
         <v>1</v>
@@ -3658,18 +3660,18 @@
       </c>
       <c r="S19" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M19,Trigger),"--")</f>
-        <v>42515</v>
+        <v>42550</v>
       </c>
       <c r="T19" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M19,Trigger),"--")</f>
-        <v>42699</v>
+        <v>42733</v>
       </c>
       <c r="V19" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W19" s="3" t="str">
-        <v>obj_00563</v>
+        <v>obj_00578</v>
       </c>
       <c r="X19" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W19,Trigger),"")</f>
@@ -3677,7 +3679,7 @@
       </c>
       <c r="Y19" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W19,Trigger),"")</f>
-        <v>5.6999999999999998E-4</v>
+        <v>-4.2999999999999999E-4</v>
       </c>
       <c r="Z19" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W19)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W19)),_xll.qlSwapRateHelperSpread($W19))</f>
@@ -3685,14 +3687,14 @@
       </c>
       <c r="AA19" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W19,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB19" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W19,Trigger),"")</f>
-        <v>43003</v>
+        <v>43038</v>
       </c>
       <c r="AC19" s="68">
-        <v>5.6398778210864538E-4</v>
+        <v>-4.3354105361598423E-4</v>
       </c>
       <c r="AD19" s="158"/>
       <c r="AH19" s="156"/>
@@ -3722,7 +3724,7 @@
       <c r="I20" s="121"/>
       <c r="J20" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H20,B20&amp;"M",G20,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0054b#0001</v>
+        <v>obj_00552#0000</v>
       </c>
       <c r="K20" s="48"/>
       <c r="L20" s="9" t="str">
@@ -3731,7 +3733,7 @@
       </c>
       <c r="M20" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_00546#0001</v>
+        <v>obj_00551#0000</v>
       </c>
       <c r="N20" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M20,Trigger),"--")</f>
@@ -3739,7 +3741,7 @@
       </c>
       <c r="O20" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M20,Trigger),"--")</f>
-        <v>3.0999999999999995E-4</v>
+        <v>-8.3000000000000001E-4</v>
       </c>
       <c r="P20" s="93" t="b">
         <v>1</v>
@@ -3752,18 +3754,18 @@
       </c>
       <c r="S20" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M20,Trigger),"--")</f>
-        <v>42548</v>
+        <v>42580</v>
       </c>
       <c r="T20" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M20,Trigger),"--")</f>
-        <v>42731</v>
+        <v>42765</v>
       </c>
       <c r="V20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W20" s="3" t="str">
-        <v>obj_00551</v>
+        <v>obj_00562</v>
       </c>
       <c r="X20" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W20,Trigger),"")</f>
@@ -3771,7 +3773,7 @@
       </c>
       <c r="Y20" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W20,Trigger),"")</f>
-        <v>1.2800000000000001E-3</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="Z20" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W20)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W20)),_xll.qlSwapRateHelperSpread($W20))</f>
@@ -3779,14 +3781,14 @@
       </c>
       <c r="AA20" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W20,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB20" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W20,Trigger),"")</f>
-        <v>43368</v>
+        <v>43402</v>
       </c>
       <c r="AC20" s="68">
-        <v>1.2743102179329309E-3</v>
+        <v>1.2393256948018034E-4</v>
       </c>
       <c r="AD20" s="158"/>
       <c r="AH20" s="156"/>
@@ -3816,7 +3818,7 @@
       <c r="I21" s="121"/>
       <c r="J21" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H21,B21&amp;"M",G21,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0054a#0001</v>
+        <v>obj_0054f#0000</v>
       </c>
       <c r="K21" s="48"/>
       <c r="L21" s="9" t="str">
@@ -3825,7 +3827,7 @@
       </c>
       <c r="M21" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_0054d#0001</v>
+        <v>obj_00550#0000</v>
       </c>
       <c r="N21" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M21,Trigger),"--")</f>
@@ -3833,7 +3835,7 @@
       </c>
       <c r="O21" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M21,Trigger),"--")</f>
-        <v>3.5999999999999997E-4</v>
+        <v>-8.3000000000000001E-4</v>
       </c>
       <c r="P21" s="93" t="b">
         <v>1</v>
@@ -3846,18 +3848,18 @@
       </c>
       <c r="S21" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M21,Trigger),"--")</f>
-        <v>42576</v>
+        <v>42611</v>
       </c>
       <c r="T21" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M21,Trigger),"--")</f>
-        <v>42760</v>
+        <v>42794</v>
       </c>
       <c r="V21" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W21" s="3" t="str">
-        <v>obj_00552</v>
+        <v>obj_00565</v>
       </c>
       <c r="X21" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W21,Trigger),"")</f>
@@ -3865,7 +3867,7 @@
       </c>
       <c r="Y21" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W21,Trigger),"")</f>
-        <v>2.3899999999999998E-3</v>
+        <v>1.1100000000000001E-3</v>
       </c>
       <c r="Z21" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W21)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W21)),_xll.qlSwapRateHelperSpread($W21))</f>
@@ -3873,14 +3875,14 @@
       </c>
       <c r="AA21" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W21,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB21" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W21,Trigger),"")</f>
-        <v>43733</v>
+        <v>43767</v>
       </c>
       <c r="AC21" s="68">
-        <v>2.3858676021284993E-3</v>
+        <v>1.1055325543293793E-3</v>
       </c>
       <c r="AD21" s="158"/>
       <c r="AH21" s="156"/>
@@ -3910,7 +3912,7 @@
       <c r="I22" s="121"/>
       <c r="J22" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H22,B22&amp;"M",G22,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00546#0001</v>
+        <v>obj_00551#0000</v>
       </c>
       <c r="K22" s="48"/>
       <c r="L22" s="9" t="str">
@@ -3919,7 +3921,7 @@
       </c>
       <c r="M22" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_00549#0001</v>
+        <v>obj_00554#0000</v>
       </c>
       <c r="N22" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M22,Trigger),"--")</f>
@@ -3927,7 +3929,7 @@
       </c>
       <c r="O22" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M22,Trigger),"--")</f>
-        <v>4.0999999999999994E-4</v>
+        <v>-8.0000000000000015E-4</v>
       </c>
       <c r="P22" s="93" t="b">
         <v>1</v>
@@ -3940,18 +3942,18 @@
       </c>
       <c r="S22" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M22,Trigger),"--")</f>
-        <v>42607</v>
+        <v>42642</v>
       </c>
       <c r="T22" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M22,Trigger),"--")</f>
-        <v>42793</v>
+        <v>42823</v>
       </c>
       <c r="V22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W22" s="3" t="str">
-        <v>obj_00558</v>
+        <v>obj_0055e</v>
       </c>
       <c r="X22" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W22,Trigger),"")</f>
@@ -3959,7 +3961,7 @@
       </c>
       <c r="Y22" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W22,Trigger),"")</f>
-        <v>3.6800000000000001E-3</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="Z22" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W22)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W22)),_xll.qlSwapRateHelperSpread($W22))</f>
@@ -3967,14 +3969,14 @@
       </c>
       <c r="AA22" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W22,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB22" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W22,Trigger),"")</f>
-        <v>44099</v>
+        <v>44133</v>
       </c>
       <c r="AC22" s="68">
-        <v>3.6799743322419791E-3</v>
+        <v>2.2688749243109465E-3</v>
       </c>
       <c r="AD22" s="158"/>
       <c r="AH22" s="156"/>
@@ -4004,7 +4006,7 @@
       <c r="I23" s="121"/>
       <c r="J23" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H23,B23&amp;"M",G23,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0054d#0001</v>
+        <v>obj_00550#0000</v>
       </c>
       <c r="K23" s="48"/>
       <c r="L23" s="9" t="str">
@@ -4013,7 +4015,7 @@
       </c>
       <c r="M23" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_00547#0001</v>
+        <v>obj_00553#0000</v>
       </c>
       <c r="N23" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M23,Trigger),"--")</f>
@@ -4021,7 +4023,7 @@
       </c>
       <c r="O23" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M23,Trigger),"--")</f>
-        <v>4.6999999999999999E-4</v>
+        <v>-7.400000000000001E-4</v>
       </c>
       <c r="P23" s="93" t="b">
         <v>1</v>
@@ -4034,18 +4036,18 @@
       </c>
       <c r="S23" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M23,Trigger),"--")</f>
-        <v>42639</v>
+        <v>42674</v>
       </c>
       <c r="T23" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M23,Trigger),"--")</f>
-        <v>42821</v>
+        <v>42853</v>
       </c>
       <c r="V23" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W23" s="3" t="str">
-        <v>obj_00550</v>
+        <v>obj_0055d</v>
       </c>
       <c r="X23" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W23,Trigger),"")</f>
@@ -4053,7 +4055,7 @@
       </c>
       <c r="Y23" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W23,Trigger),"")</f>
-        <v>5.0200000000000002E-3</v>
+        <v>3.5099999999999997E-3</v>
       </c>
       <c r="Z23" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W23)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W23)),_xll.qlSwapRateHelperSpread($W23))</f>
@@ -4061,14 +4063,14 @@
       </c>
       <c r="AA23" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W23,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB23" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W23,Trigger),"")</f>
-        <v>44466</v>
+        <v>44498</v>
       </c>
       <c r="AC23" s="68">
-        <v>5.0325598204600868E-3</v>
+        <v>3.5183213104680502E-3</v>
       </c>
       <c r="AD23" s="158"/>
       <c r="AH23" s="156"/>
@@ -4098,7 +4100,7 @@
       <c r="I24" s="121"/>
       <c r="J24" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H24,B24&amp;"M",G24,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00549#0001</v>
+        <v>obj_00554#0000</v>
       </c>
       <c r="K24" s="48"/>
       <c r="L24" s="9" t="str">
@@ -4139,7 +4141,7 @@
         <v>Sw</v>
       </c>
       <c r="W24" s="3" t="str">
-        <v>obj_0056d</v>
+        <v>obj_0055b</v>
       </c>
       <c r="X24" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W24,Trigger),"")</f>
@@ -4147,7 +4149,7 @@
       </c>
       <c r="Y24" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W24,Trigger),"")</f>
-        <v>6.3599999999999993E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="Z24" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W24)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W24)),_xll.qlSwapRateHelperSpread($W24))</f>
@@ -4155,14 +4157,14 @@
       </c>
       <c r="AA24" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W24,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB24" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W24,Trigger),"")</f>
-        <v>44830</v>
+        <v>44865</v>
       </c>
       <c r="AC24" s="68">
-        <v>6.3934949910536389E-3</v>
+        <v>4.8253190912867098E-3</v>
       </c>
       <c r="AD24" s="158"/>
       <c r="AH24" s="156"/>
@@ -4192,7 +4194,7 @@
       <c r="I25" s="121"/>
       <c r="J25" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H25,B25&amp;"M",G25,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00547#0001</v>
+        <v>obj_00553#0000</v>
       </c>
       <c r="K25" s="48"/>
       <c r="L25" s="9" t="str">
@@ -4233,7 +4235,7 @@
         <v>Sw</v>
       </c>
       <c r="W25" s="3" t="str">
-        <v>obj_0055d</v>
+        <v>obj_00573</v>
       </c>
       <c r="X25" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W25,Trigger),"")</f>
@@ -4241,7 +4243,7 @@
       </c>
       <c r="Y25" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W25,Trigger),"")</f>
-        <v>7.6499999999999988E-3</v>
+        <v>6.0499999999999998E-3</v>
       </c>
       <c r="Z25" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W25)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W25)),_xll.qlSwapRateHelperSpread($W25))</f>
@@ -4249,14 +4251,14 @@
       </c>
       <c r="AA25" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W25,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB25" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W25,Trigger),"")</f>
-        <v>45194</v>
+        <v>45229</v>
       </c>
       <c r="AC25" s="68">
-        <v>7.7130914398423995E-3</v>
+        <v>6.1022263821107654E-3</v>
       </c>
       <c r="AD25" s="158"/>
       <c r="AH25" s="156"/>
@@ -4292,7 +4294,7 @@
       </c>
       <c r="M26" s="90" t="str">
         <f t="shared" si="8"/>
-        <v>obj_00548#0001</v>
+        <v>obj_0054d#0000</v>
       </c>
       <c r="N26" s="143" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M26,Trigger),"--")</f>
@@ -4300,7 +4302,7 @@
       </c>
       <c r="O26" s="94">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M26,Trigger),"--")</f>
-        <v>7.6000000000000015E-4</v>
+        <v>-5.2999999999999998E-4</v>
       </c>
       <c r="P26" s="93" t="b">
         <v>1</v>
@@ -4313,18 +4315,18 @@
       </c>
       <c r="S26" s="95">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M26,Trigger),"--")</f>
-        <v>42731</v>
+        <v>42765</v>
       </c>
       <c r="T26" s="95">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M26,Trigger),"--")</f>
-        <v>42912</v>
+        <v>42947</v>
       </c>
       <c r="V26" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Sw</v>
       </c>
       <c r="W26" s="3" t="str">
-        <v>obj_00567</v>
+        <v>obj_00564</v>
       </c>
       <c r="X26" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W26,Trigger),"")</f>
@@ -4332,7 +4334,7 @@
       </c>
       <c r="Y26" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W26,Trigger),"")</f>
-        <v>8.8400000000000006E-3</v>
+        <v>7.2099999999999994E-3</v>
       </c>
       <c r="Z26" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W26)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W26)),_xll.qlSwapRateHelperSpread($W26))</f>
@@ -4340,14 +4342,14 @@
       </c>
       <c r="AA26" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W26,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB26" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W26,Trigger),"")</f>
-        <v>45560</v>
+        <v>45594</v>
       </c>
       <c r="AC26" s="68">
-        <v>8.9370553590686352E-3</v>
+        <v>7.2914645315025114E-3</v>
       </c>
       <c r="AD26" s="158"/>
       <c r="AH26" s="156"/>
@@ -4415,7 +4417,7 @@
         <v>Sw</v>
       </c>
       <c r="W27" s="3" t="str">
-        <v>obj_0055c</v>
+        <v>obj_00561</v>
       </c>
       <c r="X27" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W27,Trigger),"")</f>
@@ -4423,7 +4425,7 @@
       </c>
       <c r="Y27" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W27,Trigger),"")</f>
-        <v>9.8999999999999991E-3</v>
+        <v>8.2700000000000013E-3</v>
       </c>
       <c r="Z27" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W27)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W27)),_xll.qlSwapRateHelperSpread($W27))</f>
@@ -4431,14 +4433,14 @@
       </c>
       <c r="AA27" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W27,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB27" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W27,Trigger),"")</f>
-        <v>45925</v>
+        <v>45959</v>
       </c>
       <c r="AC27" s="68">
-        <v>1.0038075845684464E-2</v>
+        <v>8.3884498337278776E-3</v>
       </c>
       <c r="AD27" s="158"/>
       <c r="AH27" s="156"/>
@@ -4468,7 +4470,7 @@
       <c r="I28" s="121"/>
       <c r="J28" s="62" t="str">
         <f>_xll.qlFraRateHelper(,H28,B28&amp;"M",G28,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00548#0001</v>
+        <v>obj_0054d#0000</v>
       </c>
       <c r="K28" s="48"/>
       <c r="L28" s="9" t="str">
@@ -4509,7 +4511,7 @@
         <v>Sw</v>
       </c>
       <c r="W28" s="3" t="str">
-        <v>obj_00559</v>
+        <v>obj_00566</v>
       </c>
       <c r="X28" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W28,Trigger),"")</f>
@@ -4517,7 +4519,7 @@
       </c>
       <c r="Y28" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W28,Trigger),"")</f>
-        <v>1.0860000000000002E-2</v>
+        <v>9.2299999999999986E-3</v>
       </c>
       <c r="Z28" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W28)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W28)),_xll.qlSwapRateHelperSpread($W28))</f>
@@ -4525,14 +4527,14 @@
       </c>
       <c r="AA28" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W28,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB28" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W28,Trigger),"")</f>
-        <v>46290</v>
+        <v>46324</v>
       </c>
       <c r="AC28" s="68">
-        <v>1.1043282415927497E-2</v>
+        <v>9.389554086262835E-3</v>
       </c>
       <c r="AD28" s="158"/>
       <c r="AH28" s="156"/>
@@ -4600,7 +4602,7 @@
         <v>Sw</v>
       </c>
       <c r="W29" s="3" t="str">
-        <v>obj_00560</v>
+        <v>obj_00563</v>
       </c>
       <c r="X29" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W29,Trigger),"")</f>
@@ -4608,7 +4610,7 @@
       </c>
       <c r="Y29" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W29,Trigger),"")</f>
-        <v>1.171E-2</v>
+        <v>1.0089999999999998E-2</v>
       </c>
       <c r="Z29" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W29)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W29)),_xll.qlSwapRateHelperSpread($W29))</f>
@@ -4616,14 +4618,14 @@
       </c>
       <c r="AA29" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W29,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB29" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W29,Trigger),"")</f>
-        <v>46657</v>
+        <v>46689</v>
       </c>
       <c r="AC29" s="68">
-        <v>1.1939971811656423E-2</v>
+        <v>1.0293118290126052E-2</v>
       </c>
       <c r="AD29" s="158"/>
       <c r="AH29" s="156"/>
@@ -4691,7 +4693,7 @@
         <v>Sw</v>
       </c>
       <c r="W30" s="3" t="str">
-        <v>obj_00556</v>
+        <v>obj_00572</v>
       </c>
       <c r="X30" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W30,Trigger),"")</f>
@@ -4699,7 +4701,7 @@
       </c>
       <c r="Y30" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W30,Trigger),"")</f>
-        <v>1.2450000000000001E-2</v>
+        <v>1.0840000000000001E-2</v>
       </c>
       <c r="Z30" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W30)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W30)),_xll.qlSwapRateHelperSpread($W30))</f>
@@ -4707,14 +4709,14 @@
       </c>
       <c r="AA30" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W30,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB30" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W30,Trigger),"")</f>
-        <v>47021</v>
+        <v>47056</v>
       </c>
       <c r="AC30" s="68">
-        <v>1.2723429096065728E-2</v>
+        <v>1.1084120496089065E-2</v>
       </c>
       <c r="AD30" s="158"/>
       <c r="AH30" s="156"/>
@@ -4782,7 +4784,7 @@
         <v>Sw</v>
       </c>
       <c r="W31" s="3" t="str">
-        <v>obj_00561</v>
+        <v>obj_0056c</v>
       </c>
       <c r="X31" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W31,Trigger),"")</f>
@@ -4790,7 +4792,7 @@
       </c>
       <c r="Y31" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W31,Trigger),"")</f>
-        <v>1.307E-2</v>
+        <v>1.1480000000000001E-2</v>
       </c>
       <c r="Z31" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W31)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W31)),_xll.qlSwapRateHelperSpread($W31))</f>
@@ -4798,14 +4800,14 @@
       </c>
       <c r="AA31" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W31,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB31" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W31,Trigger),"")</f>
-        <v>47386</v>
+        <v>47420</v>
       </c>
       <c r="AC31" s="68">
-        <v>1.3384972619600219E-2</v>
+        <v>1.1764894927822058E-2</v>
       </c>
       <c r="AD31" s="158"/>
       <c r="AH31" s="156"/>
@@ -4861,7 +4863,7 @@
         <v>Sw</v>
       </c>
       <c r="W32" s="3" t="str">
-        <v>obj_00554</v>
+        <v>obj_0056e</v>
       </c>
       <c r="X32" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W32,Trigger),"")</f>
@@ -4869,7 +4871,7 @@
       </c>
       <c r="Y32" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W32,Trigger),"")</f>
-        <v>1.359E-2</v>
+        <v>1.204E-2</v>
       </c>
       <c r="Z32" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W32)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W32)),_xll.qlSwapRateHelperSpread($W32))</f>
@@ -4877,14 +4879,14 @@
       </c>
       <c r="AA32" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W32,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB32" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W32,Trigger),"")</f>
-        <v>47751</v>
+        <v>47785</v>
       </c>
       <c r="AC32" s="68">
-        <v>1.3941565477005001E-2</v>
+        <v>1.2363420391731404E-2</v>
       </c>
       <c r="AD32" s="158"/>
     </row>
@@ -4952,7 +4954,7 @@
         <v>Sw</v>
       </c>
       <c r="W33" s="3" t="str">
-        <v>obj_00570</v>
+        <v>obj_0056d</v>
       </c>
       <c r="X33" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W33,Trigger),"")</f>
@@ -4960,7 +4962,7 @@
       </c>
       <c r="Y33" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W33,Trigger),"")</f>
-        <v>1.4030000000000001E-2</v>
+        <v>1.252E-2</v>
       </c>
       <c r="Z33" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W33)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W33)),_xll.qlSwapRateHelperSpread($W33))</f>
@@ -4968,14 +4970,14 @@
       </c>
       <c r="AA33" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W33,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB33" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W33,Trigger),"")</f>
-        <v>48116</v>
+        <v>48150</v>
       </c>
       <c r="AC33" s="68">
-        <v>1.4413560031661849E-2</v>
+        <v>1.2878261786368609E-2</v>
       </c>
       <c r="AD33" s="158"/>
     </row>
@@ -4988,7 +4990,7 @@
       </c>
       <c r="C34" s="56" t="str">
         <f>_xll.qlIMMNextCode(Evaluationdate-1,B34,Trigger)</f>
-        <v>V5</v>
+        <v>X5</v>
       </c>
       <c r="D34" s="127"/>
       <c r="E34" s="127"/>
@@ -4999,11 +5001,11 @@
       </c>
       <c r="H34" s="114" t="str">
         <f t="shared" ref="H34:H55" si="15">Currency&amp;"FUT"&amp;$G$32&amp;$C34&amp;QuoteSuffix</f>
-        <v>EURFUT3MV5_Quote</v>
+        <v>EURFUT3MX5_Quote</v>
       </c>
       <c r="I34" s="114" t="str">
         <f t="shared" ref="I34:I55" si="16">Currency&amp;"FUT"&amp;$G$32&amp;$C34&amp;"ConvAdj"&amp;QuoteSuffix</f>
-        <v>EURFUT3MV5ConvAdj_Quote</v>
+        <v>EURFUT3MX5ConvAdj_Quote</v>
       </c>
       <c r="J34" s="57"/>
       <c r="K34" s="48"/>
@@ -5045,7 +5047,7 @@
         <v>Sw</v>
       </c>
       <c r="W34" s="3" t="str">
-        <v>obj_00564</v>
+        <v>obj_00574</v>
       </c>
       <c r="X34" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W34,Trigger),"")</f>
@@ -5053,7 +5055,7 @@
       </c>
       <c r="Y34" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W34,Trigger),"")</f>
-        <v>1.44E-2</v>
+        <v>1.2920000000000001E-2</v>
       </c>
       <c r="Z34" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W34)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W34)),_xll.qlSwapRateHelperSpread($W34))</f>
@@ -5061,14 +5063,14 @@
       </c>
       <c r="AA34" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W34,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB34" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W34,Trigger),"")</f>
-        <v>48484</v>
+        <v>48516</v>
       </c>
       <c r="AC34" s="68">
-        <v>1.4808052880090534E-2</v>
+        <v>1.3305423573717886E-2</v>
       </c>
       <c r="AD34" s="158"/>
     </row>
@@ -5081,7 +5083,7 @@
       </c>
       <c r="C35" s="61" t="str">
         <f>_xll.qlIMMNextCode(C34,B35,Trigger)</f>
-        <v>X5</v>
+        <v>Z5</v>
       </c>
       <c r="D35" s="121"/>
       <c r="E35" s="121"/>
@@ -5092,11 +5094,11 @@
       </c>
       <c r="H35" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MX5_Quote</v>
+        <v>EURFUT3MZ5_Quote</v>
       </c>
       <c r="I35" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MX5ConvAdj_Quote</v>
+        <v>EURFUT3MZ5ConvAdj_Quote</v>
       </c>
       <c r="J35" s="62"/>
       <c r="K35" s="48"/>
@@ -5138,7 +5140,7 @@
         <v>Sw</v>
       </c>
       <c r="W35" s="3" t="str">
-        <v>obj_0055a</v>
+        <v>obj_0056b</v>
       </c>
       <c r="X35" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W35,Trigger),"")</f>
@@ -5146,7 +5148,7 @@
       </c>
       <c r="Y35" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W35,Trigger),"")</f>
-        <v>1.47E-2</v>
+        <v>1.3260000000000001E-2</v>
       </c>
       <c r="Z35" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W35)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W35)),_xll.qlSwapRateHelperSpread($W35))</f>
@@ -5154,14 +5156,14 @@
       </c>
       <c r="AA35" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W35,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB35" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W35,Trigger),"")</f>
-        <v>48848</v>
+        <v>48883</v>
       </c>
       <c r="AC35" s="68">
-        <v>1.5128599784086018E-2</v>
+        <v>1.367036592204395E-2</v>
       </c>
       <c r="AD35" s="158"/>
     </row>
@@ -5174,7 +5176,7 @@
       </c>
       <c r="C36" s="61" t="str">
         <f>_xll.qlIMMNextCode(C35,B36,Trigger)</f>
-        <v>Z5</v>
+        <v>F6</v>
       </c>
       <c r="D36" s="121"/>
       <c r="E36" s="121"/>
@@ -5185,11 +5187,11 @@
       </c>
       <c r="H36" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MZ5_Quote</v>
+        <v>EURFUT3MF6_Quote</v>
       </c>
       <c r="I36" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MZ5ConvAdj_Quote</v>
+        <v>EURFUT3MF6ConvAdj_Quote</v>
       </c>
       <c r="J36" s="62"/>
       <c r="K36" s="48"/>
@@ -5239,7 +5241,7 @@
       </c>
       <c r="Y36" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W36,Trigger),"")</f>
-        <v>1.4929999999999999E-2</v>
+        <v>1.3540000000000002E-2</v>
       </c>
       <c r="Z36" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W36)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W36)),_xll.qlSwapRateHelperSpread($W36))</f>
@@ -5247,14 +5249,14 @@
       </c>
       <c r="AA36" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W36,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB36" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W36,Trigger),"")</f>
-        <v>49212</v>
+        <v>49247</v>
       </c>
       <c r="AC36" s="68">
-        <v>1.5370878384669894E-2</v>
+        <v>1.3972006490708191E-2</v>
       </c>
       <c r="AD36" s="158"/>
     </row>
@@ -5267,7 +5269,7 @@
       </c>
       <c r="C37" s="61" t="str">
         <f>_xll.qlIMMNextCode(C36,B37,Trigger)</f>
-        <v>F6</v>
+        <v>G6</v>
       </c>
       <c r="D37" s="121"/>
       <c r="E37" s="121"/>
@@ -5278,11 +5280,11 @@
       </c>
       <c r="H37" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MF6_Quote</v>
+        <v>EURFUT3MG6_Quote</v>
       </c>
       <c r="I37" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MF6ConvAdj_Quote</v>
+        <v>EURFUT3MG6ConvAdj_Quote</v>
       </c>
       <c r="J37" s="62"/>
       <c r="K37" s="48"/>
@@ -5324,7 +5326,7 @@
         <v>Sw</v>
       </c>
       <c r="W37" s="3" t="str">
-        <v>obj_0056e</v>
+        <v>obj_00576</v>
       </c>
       <c r="X37" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W37,Trigger),"")</f>
@@ -5332,7 +5334,7 @@
       </c>
       <c r="Y37" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W37,Trigger),"")</f>
-        <v>1.5110000000000002E-2</v>
+        <v>1.375E-2</v>
       </c>
       <c r="Z37" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W37)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W37)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W37)),_xll.qlSwapRateHelperSpread($W37))</f>
@@ -5340,14 +5342,14 @@
       </c>
       <c r="AA37" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W37,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB37" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W37,Trigger),"")</f>
-        <v>49577</v>
+        <v>49611</v>
       </c>
       <c r="AC37" s="68">
-        <v>1.5557122359418132E-2</v>
+        <v>1.4192903543022013E-2</v>
       </c>
       <c r="AD37" s="158"/>
     </row>
@@ -5360,7 +5362,7 @@
       </c>
       <c r="C38" s="8" t="str">
         <f>_xll.qlIMMNextCode(C37,B38,Trigger)</f>
-        <v>G6</v>
+        <v>H6</v>
       </c>
       <c r="D38" s="122"/>
       <c r="E38" s="122"/>
@@ -5371,11 +5373,11 @@
       </c>
       <c r="H38" s="116" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MG6_Quote</v>
+        <v>EURFUT3MH6_Quote</v>
       </c>
       <c r="I38" s="116" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MG6ConvAdj_Quote</v>
+        <v>EURFUT3MH6ConvAdj_Quote</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="48"/>
@@ -5425,7 +5427,7 @@
       </c>
       <c r="Y38" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W38,Trigger),"")</f>
-        <v>1.525E-2</v>
+        <v>1.3919999999999998E-2</v>
       </c>
       <c r="Z38" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W38)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W38)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W38)),_xll.qlSwapRateHelperSpread($W38))</f>
@@ -5433,14 +5435,14 @@
       </c>
       <c r="AA38" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W38,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB38" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W38,Trigger),"")</f>
-        <v>49943</v>
+        <v>49977</v>
       </c>
       <c r="AC38" s="68">
-        <v>1.5696332639462712E-2</v>
+        <v>1.4367168987590368E-2</v>
       </c>
       <c r="AD38" s="158"/>
     </row>
@@ -5453,7 +5455,7 @@
       </c>
       <c r="C39" s="61" t="str">
         <f>_xll.qlIMMNextCode(C38,B39,Trigger)</f>
-        <v>H6</v>
+        <v>M6</v>
       </c>
       <c r="D39" s="121"/>
       <c r="E39" s="121"/>
@@ -5464,11 +5466,11 @@
       </c>
       <c r="H39" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MH6_Quote</v>
+        <v>EURFUT3MM6_Quote</v>
       </c>
       <c r="I39" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MH6ConvAdj_Quote</v>
+        <v>EURFUT3MM6ConvAdj_Quote</v>
       </c>
       <c r="J39" s="62"/>
       <c r="L39" s="9" t="str">
@@ -5509,7 +5511,7 @@
         <v>Sw</v>
       </c>
       <c r="W39" s="3" t="str">
-        <v>obj_0056b</v>
+        <v>obj_0055c</v>
       </c>
       <c r="X39" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W39,Trigger),"")</f>
@@ -5517,7 +5519,7 @@
       </c>
       <c r="Y39" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W39,Trigger),"")</f>
-        <v>1.5339999999999999E-2</v>
+        <v>1.4039999999999999E-2</v>
       </c>
       <c r="Z39" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W39)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W39)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W39)),_xll.qlSwapRateHelperSpread($W39))</f>
@@ -5525,14 +5527,14 @@
       </c>
       <c r="AA39" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W39,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB39" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W39,Trigger),"")</f>
-        <v>50308</v>
+        <v>50342</v>
       </c>
       <c r="AC39" s="68">
-        <v>1.5779749810578801E-2</v>
+        <v>1.4486119824693009E-2</v>
       </c>
       <c r="AD39" s="158"/>
     </row>
@@ -5545,7 +5547,7 @@
       </c>
       <c r="C40" s="61" t="str">
         <f>_xll.qlIMMNextCode(C39,B40,Trigger)</f>
-        <v>M6</v>
+        <v>U6</v>
       </c>
       <c r="D40" s="121"/>
       <c r="E40" s="121"/>
@@ -5556,11 +5558,11 @@
       </c>
       <c r="H40" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MM6_Quote</v>
+        <v>EURFUT3MU6_Quote</v>
       </c>
       <c r="I40" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MM6ConvAdj_Quote</v>
+        <v>EURFUT3MU6ConvAdj_Quote</v>
       </c>
       <c r="J40" s="62"/>
       <c r="L40" s="9" t="str">
@@ -5601,7 +5603,7 @@
         <v>Sw</v>
       </c>
       <c r="W40" s="3" t="str">
-        <v>obj_0056c</v>
+        <v>obj_00575</v>
       </c>
       <c r="X40" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W40,Trigger),"")</f>
@@ -5609,7 +5611,7 @@
       </c>
       <c r="Y40" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W40,Trigger),"")</f>
-        <v>1.541E-2</v>
+        <v>1.4119999999999999E-2</v>
       </c>
       <c r="Z40" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W40)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W40)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W40)),_xll.qlSwapRateHelperSpread($W40))</f>
@@ -5617,14 +5619,14 @@
       </c>
       <c r="AA40" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W40,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB40" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W40,Trigger),"")</f>
-        <v>50675</v>
+        <v>50707</v>
       </c>
       <c r="AC40" s="68">
-        <v>1.5840918221787438E-2</v>
+        <v>1.4559033373344249E-2</v>
       </c>
       <c r="AD40" s="158"/>
     </row>
@@ -5637,7 +5639,7 @@
       </c>
       <c r="C41" s="61" t="str">
         <f>_xll.qlIMMNextCode(C40,B41,Trigger)</f>
-        <v>U6</v>
+        <v>Z6</v>
       </c>
       <c r="D41" s="121"/>
       <c r="E41" s="121"/>
@@ -5648,11 +5650,11 @@
       </c>
       <c r="H41" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MU6_Quote</v>
+        <v>EURFUT3MZ6_Quote</v>
       </c>
       <c r="I41" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MU6ConvAdj_Quote</v>
+        <v>EURFUT3MZ6ConvAdj_Quote</v>
       </c>
       <c r="J41" s="62"/>
       <c r="L41" s="9" t="str">
@@ -5693,7 +5695,7 @@
         <v>Sw</v>
       </c>
       <c r="W41" s="3" t="str">
-        <v>obj_00571</v>
+        <v>obj_00577</v>
       </c>
       <c r="X41" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W41,Trigger),"")</f>
@@ -5701,7 +5703,7 @@
       </c>
       <c r="Y41" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W41,Trigger),"")</f>
-        <v>1.5449999999999998E-2</v>
+        <v>1.4180000000000002E-2</v>
       </c>
       <c r="Z41" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W41)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W41)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W41)),_xll.qlSwapRateHelperSpread($W41))</f>
@@ -5709,14 +5711,14 @@
       </c>
       <c r="AA41" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W41,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB41" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W41,Trigger),"")</f>
-        <v>51039</v>
+        <v>51074</v>
       </c>
       <c r="AC41" s="68">
-        <v>1.5867364809753454E-2</v>
+        <v>1.4609507670442137E-2</v>
       </c>
       <c r="AD41" s="158"/>
     </row>
@@ -5729,7 +5731,7 @@
       </c>
       <c r="C42" s="61" t="str">
         <f>_xll.qlIMMNextCode(C41,B42,Trigger)</f>
-        <v>Z6</v>
+        <v>H7</v>
       </c>
       <c r="D42" s="121"/>
       <c r="E42" s="121"/>
@@ -5740,11 +5742,11 @@
       </c>
       <c r="H42" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MZ6_Quote</v>
+        <v>EURFUT3MH7_Quote</v>
       </c>
       <c r="I42" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MZ6ConvAdj_Quote</v>
+        <v>EURFUT3MH7ConvAdj_Quote</v>
       </c>
       <c r="J42" s="62"/>
       <c r="L42" s="9" t="str">
@@ -5785,7 +5787,7 @@
         <v>Sw</v>
       </c>
       <c r="W42" s="3" t="str">
-        <v>obj_0056a</v>
+        <v>obj_00571</v>
       </c>
       <c r="X42" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W42,Trigger),"")</f>
@@ -5793,7 +5795,7 @@
       </c>
       <c r="Y42" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W42,Trigger),"")</f>
-        <v>1.5480000000000001E-2</v>
+        <v>1.423E-2</v>
       </c>
       <c r="Z42" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W42)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W42)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W42)),_xll.qlSwapRateHelperSpread($W42))</f>
@@ -5801,14 +5803,14 @@
       </c>
       <c r="AA42" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W42,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB42" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W42,Trigger),"")</f>
-        <v>51404</v>
+        <v>51438</v>
       </c>
       <c r="AC42" s="68">
-        <v>1.5881478717459478E-2</v>
+        <v>1.4649717696647722E-2</v>
       </c>
       <c r="AD42" s="158"/>
     </row>
@@ -5821,7 +5823,7 @@
       </c>
       <c r="C43" s="61" t="str">
         <f>_xll.qlIMMNextCode(C42,B43,Trigger)</f>
-        <v>H7</v>
+        <v>M7</v>
       </c>
       <c r="D43" s="121"/>
       <c r="E43" s="121"/>
@@ -5832,11 +5834,11 @@
       </c>
       <c r="H43" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MH7_Quote</v>
+        <v>EURFUT3MM7_Quote</v>
       </c>
       <c r="I43" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MH7ConvAdj_Quote</v>
+        <v>EURFUT3MM7ConvAdj_Quote</v>
       </c>
       <c r="J43" s="62"/>
       <c r="L43" s="9" t="str">
@@ -5877,7 +5879,7 @@
         <v>Sw</v>
       </c>
       <c r="W43" s="3" t="str">
-        <v>obj_00553</v>
+        <v>obj_0056a</v>
       </c>
       <c r="X43" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W43,Trigger),"")</f>
@@ -5885,7 +5887,7 @@
       </c>
       <c r="Y43" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W43,Trigger),"")</f>
-        <v>1.55E-2</v>
+        <v>1.427E-2</v>
       </c>
       <c r="Z43" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W43)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W43)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W43)),_xll.qlSwapRateHelperSpread($W43))</f>
@@ -5893,14 +5895,14 @@
       </c>
       <c r="AA43" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W43,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB43" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W43,Trigger),"")</f>
-        <v>51769</v>
+        <v>51803</v>
       </c>
       <c r="AC43" s="68">
-        <v>1.5886486222587048E-2</v>
+        <v>1.4679112866378451E-2</v>
       </c>
       <c r="AD43" s="158"/>
     </row>
@@ -5913,7 +5915,7 @@
       </c>
       <c r="C44" s="61" t="str">
         <f>_xll.qlIMMNextCode(C43,B44,Trigger)</f>
-        <v>M7</v>
+        <v>U7</v>
       </c>
       <c r="D44" s="121"/>
       <c r="E44" s="121"/>
@@ -5924,11 +5926,11 @@
       </c>
       <c r="H44" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MM7_Quote</v>
+        <v>EURFUT3MU7_Quote</v>
       </c>
       <c r="I44" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MM7ConvAdj_Quote</v>
+        <v>EURFUT3MU7ConvAdj_Quote</v>
       </c>
       <c r="J44" s="62"/>
       <c r="L44" s="9" t="str">
@@ -5969,7 +5971,7 @@
         <v>Sw</v>
       </c>
       <c r="W44" s="3" t="str">
-        <v>obj_00569</v>
+        <v>obj_00560</v>
       </c>
       <c r="X44" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W44,Trigger),"")</f>
@@ -5977,7 +5979,7 @@
       </c>
       <c r="Y44" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W44,Trigger),"")</f>
-        <v>1.5509999999999999E-2</v>
+        <v>1.43E-2</v>
       </c>
       <c r="Z44" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W44)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W44)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W44)),_xll.qlSwapRateHelperSpread($W44))</f>
@@ -5985,14 +5987,14 @@
       </c>
       <c r="AA44" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W44,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB44" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W44,Trigger),"")</f>
-        <v>52134</v>
+        <v>52168</v>
       </c>
       <c r="AC44" s="68">
-        <v>1.5880375293862679E-2</v>
+        <v>1.4697547422084428E-2</v>
       </c>
       <c r="AD44" s="158"/>
     </row>
@@ -6005,7 +6007,7 @@
       </c>
       <c r="C45" s="61" t="str">
         <f>_xll.qlIMMNextCode(C44,B45,Trigger)</f>
-        <v>U7</v>
+        <v>Z7</v>
       </c>
       <c r="D45" s="121"/>
       <c r="E45" s="121"/>
@@ -6016,11 +6018,11 @@
       </c>
       <c r="H45" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MU7_Quote</v>
+        <v>EURFUT3MZ7_Quote</v>
       </c>
       <c r="I45" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MU7ConvAdj_Quote</v>
+        <v>EURFUT3MZ7ConvAdj_Quote</v>
       </c>
       <c r="J45" s="62"/>
       <c r="L45" s="9" t="str">
@@ -6061,7 +6063,7 @@
         <v>Sw</v>
       </c>
       <c r="W45" s="3" t="str">
-        <v>obj_00565</v>
+        <v>obj_00559</v>
       </c>
       <c r="X45" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W45,Trigger),"")</f>
@@ -6069,7 +6071,7 @@
       </c>
       <c r="Y45" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W45,Trigger),"")</f>
-        <v>1.5520000000000001E-2</v>
+        <v>1.4339999999999999E-2</v>
       </c>
       <c r="Z45" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W45)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W45)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W45)),_xll.qlSwapRateHelperSpread($W45))</f>
@@ -6077,14 +6079,14 @@
       </c>
       <c r="AA45" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W45,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB45" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W45,Trigger),"")</f>
-        <v>52499</v>
+        <v>52533</v>
       </c>
       <c r="AC45" s="68">
-        <v>1.5875595642748624E-2</v>
+        <v>1.4729862507328859E-2</v>
       </c>
       <c r="AD45" s="158"/>
     </row>
@@ -6097,7 +6099,7 @@
       </c>
       <c r="C46" s="61" t="str">
         <f>_xll.qlIMMNextCode(C45,B46,Trigger)</f>
-        <v>Z7</v>
+        <v>H8</v>
       </c>
       <c r="D46" s="121"/>
       <c r="E46" s="121"/>
@@ -6108,11 +6110,11 @@
       </c>
       <c r="H46" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MZ7_Quote</v>
+        <v>EURFUT3MH8_Quote</v>
       </c>
       <c r="I46" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MZ7ConvAdj_Quote</v>
+        <v>EURFUT3MH8ConvAdj_Quote</v>
       </c>
       <c r="J46" s="62"/>
       <c r="L46" s="9" t="str">
@@ -6153,7 +6155,7 @@
         <v>Sw</v>
       </c>
       <c r="W46" s="3" t="str">
-        <v>obj_00555</v>
+        <v>obj_00569</v>
       </c>
       <c r="X46" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W46,Trigger),"")</f>
@@ -6161,7 +6163,7 @@
       </c>
       <c r="Y46" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W46,Trigger),"")</f>
-        <v>1.5529999999999999E-2</v>
+        <v>1.4370000000000001E-2</v>
       </c>
       <c r="Z46" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W46)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W46)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W46)),_xll.qlSwapRateHelperSpread($W46))</f>
@@ -6169,14 +6171,14 @@
       </c>
       <c r="AA46" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W46,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB46" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W46,Trigger),"")</f>
-        <v>52866</v>
+        <v>52901</v>
       </c>
       <c r="AC46" s="68">
-        <v>1.5870485692922601E-2</v>
+        <v>1.4749330788525949E-2</v>
       </c>
       <c r="AD46" s="158"/>
     </row>
@@ -6189,7 +6191,7 @@
       </c>
       <c r="C47" s="61" t="str">
         <f>_xll.qlIMMNextCode(C46,B47,Trigger)</f>
-        <v>H8</v>
+        <v>M8</v>
       </c>
       <c r="D47" s="121"/>
       <c r="E47" s="121"/>
@@ -6200,11 +6202,11 @@
       </c>
       <c r="H47" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MH8_Quote</v>
+        <v>EURFUT3MM8_Quote</v>
       </c>
       <c r="I47" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MH8ConvAdj_Quote</v>
+        <v>EURFUT3MM8ConvAdj_Quote</v>
       </c>
       <c r="J47" s="62"/>
       <c r="L47" s="9" t="str">
@@ -6245,7 +6247,7 @@
         <v>Sw</v>
       </c>
       <c r="W47" s="3" t="str">
-        <v>obj_00568</v>
+        <v>obj_00567</v>
       </c>
       <c r="X47" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W47,Trigger),"")</f>
@@ -6253,7 +6255,7 @@
       </c>
       <c r="Y47" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W47,Trigger),"")</f>
-        <v>1.554E-2</v>
+        <v>1.439E-2</v>
       </c>
       <c r="Z47" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W47)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W47)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W47)),_xll.qlSwapRateHelperSpread($W47))</f>
@@ -6261,14 +6263,14 @@
       </c>
       <c r="AA47" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W47,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB47" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W47,Trigger),"")</f>
-        <v>53230</v>
+        <v>53265</v>
       </c>
       <c r="AC47" s="68">
-        <v>1.5868084162104348E-2</v>
+        <v>1.4760069607574746E-2</v>
       </c>
       <c r="AD47" s="158"/>
     </row>
@@ -6281,7 +6283,7 @@
       </c>
       <c r="C48" s="61" t="str">
         <f>_xll.qlIMMNextCode(C47,B48,Trigger)</f>
-        <v>M8</v>
+        <v>U8</v>
       </c>
       <c r="D48" s="121"/>
       <c r="E48" s="121"/>
@@ -6292,11 +6294,11 @@
       </c>
       <c r="H48" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MM8_Quote</v>
+        <v>EURFUT3MU8_Quote</v>
       </c>
       <c r="I48" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MM8ConvAdj_Quote</v>
+        <v>EURFUT3MU8ConvAdj_Quote</v>
       </c>
       <c r="J48" s="62"/>
       <c r="L48" s="9" t="str">
@@ -6337,7 +6339,7 @@
         <v>Sw</v>
       </c>
       <c r="W48" s="3" t="str">
-        <v>obj_00562</v>
+        <v>obj_00570</v>
       </c>
       <c r="X48" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W48,Trigger),"")</f>
@@ -6345,7 +6347,7 @@
       </c>
       <c r="Y48" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W48,Trigger),"")</f>
-        <v>1.5600000000000001E-2</v>
+        <v>1.4490000000000001E-2</v>
       </c>
       <c r="Z48" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W48)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W48)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W48)),_xll.qlSwapRateHelperSpread($W48))</f>
@@ -6353,14 +6355,14 @@
       </c>
       <c r="AA48" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W48,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB48" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W48,Trigger),"")</f>
-        <v>55057</v>
+        <v>55092</v>
       </c>
       <c r="AC48" s="68">
-        <v>1.5880849414669714E-2</v>
+        <v>1.4819665520719989E-2</v>
       </c>
       <c r="AD48" s="158"/>
     </row>
@@ -6373,7 +6375,7 @@
       </c>
       <c r="C49" s="61" t="str">
         <f>_xll.qlIMMNextCode(C48,B49,Trigger)</f>
-        <v>U8</v>
+        <v>Z8</v>
       </c>
       <c r="D49" s="121"/>
       <c r="E49" s="121"/>
@@ -6384,11 +6386,11 @@
       </c>
       <c r="H49" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MU8_Quote</v>
+        <v>EURFUT3MZ8_Quote</v>
       </c>
       <c r="I49" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MU8ConvAdj_Quote</v>
+        <v>EURFUT3MZ8ConvAdj_Quote</v>
       </c>
       <c r="J49" s="62"/>
       <c r="L49" s="9" t="str">
@@ -6429,7 +6431,7 @@
         <v>Sw</v>
       </c>
       <c r="W49" s="3" t="str">
-        <v>obj_0055e</v>
+        <v>obj_00558</v>
       </c>
       <c r="X49" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W49,Trigger),"")</f>
@@ -6437,7 +6439,7 @@
       </c>
       <c r="Y49" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W49,Trigger),"")</f>
-        <v>1.5600000000000001E-2</v>
+        <v>1.4499999999999999E-2</v>
       </c>
       <c r="Z49" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W49)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W49)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W49)),_xll.qlSwapRateHelperSpread($W49))</f>
@@ -6445,14 +6447,14 @@
       </c>
       <c r="AA49" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W49,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB49" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W49,Trigger),"")</f>
-        <v>56884</v>
+        <v>56916</v>
       </c>
       <c r="AC49" s="68">
-        <v>1.58295335123078E-2</v>
+        <v>1.4778785351152254E-2</v>
       </c>
       <c r="AD49" s="158"/>
     </row>
@@ -6465,7 +6467,7 @@
       </c>
       <c r="C50" s="61" t="str">
         <f>_xll.qlIMMNextCode(C49,B50,Trigger)</f>
-        <v>Z8</v>
+        <v>H9</v>
       </c>
       <c r="D50" s="121"/>
       <c r="E50" s="121"/>
@@ -6476,11 +6478,11 @@
       </c>
       <c r="H50" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MZ8_Quote</v>
+        <v>EURFUT3MH9_Quote</v>
       </c>
       <c r="I50" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MZ8ConvAdj_Quote</v>
+        <v>EURFUT3MH9ConvAdj_Quote</v>
       </c>
       <c r="J50" s="62"/>
       <c r="L50" s="9" t="str">
@@ -6521,7 +6523,7 @@
         <v>Sw</v>
       </c>
       <c r="W50" s="3" t="str">
-        <v>obj_0055b</v>
+        <v>obj_0056f</v>
       </c>
       <c r="X50" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W50,Trigger),"")</f>
@@ -6529,7 +6531,7 @@
       </c>
       <c r="Y50" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W50,Trigger),"")</f>
-        <v>1.5169999999999999E-2</v>
+        <v>1.4079999999999999E-2</v>
       </c>
       <c r="Z50" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W50)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W50)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W50)),_xll.qlSwapRateHelperSpread($W50))</f>
@@ -6537,14 +6539,14 @@
       </c>
       <c r="AA50" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W50,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB50" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W50,Trigger),"")</f>
-        <v>60535</v>
+        <v>60569</v>
       </c>
       <c r="AC50" s="68">
-        <v>1.5154634142301103E-2</v>
+        <v>1.412375649670619E-2</v>
       </c>
       <c r="AD50" s="158"/>
     </row>
@@ -6557,7 +6559,7 @@
       </c>
       <c r="C51" s="61" t="str">
         <f>_xll.qlIMMNextCode(C50,B51,Trigger)</f>
-        <v>H9</v>
+        <v>M9</v>
       </c>
       <c r="D51" s="121"/>
       <c r="E51" s="121"/>
@@ -6568,11 +6570,11 @@
       </c>
       <c r="H51" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MH9_Quote</v>
+        <v>EURFUT3MM9_Quote</v>
       </c>
       <c r="I51" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MH9ConvAdj_Quote</v>
+        <v>EURFUT3MM9ConvAdj_Quote</v>
       </c>
       <c r="J51" s="62"/>
       <c r="L51" s="10" t="str">
@@ -6613,7 +6615,7 @@
         <v>Sw</v>
       </c>
       <c r="W51" s="3" t="str">
-        <v>obj_0056f</v>
+        <v>obj_00568</v>
       </c>
       <c r="X51" s="3" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(W51,Trigger),"")</f>
@@ -6621,7 +6623,7 @@
       </c>
       <c r="Y51" s="68">
         <f>IFERROR(_xll.qlRateHelperRate(W51,Trigger),"")</f>
-        <v>1.502E-2</v>
+        <v>1.393E-2</v>
       </c>
       <c r="Z51" s="100">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($W51)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($W51)),"",_xll.qlFuturesRateHelperConvexityAdjustment($W51)),_xll.qlSwapRateHelperSpread($W51))</f>
@@ -6629,14 +6631,14 @@
       </c>
       <c r="AA51" s="4">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(W51,Trigger),"")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="AB51" s="4">
         <f>IFERROR(_xll.qlRateHelperPillarDate(W51,Trigger),"")</f>
-        <v>64187</v>
+        <v>64221</v>
       </c>
       <c r="AC51" s="68">
-        <v>1.4912746718746822E-2</v>
+        <v>1.3881776627150282E-2</v>
       </c>
       <c r="AD51" s="158"/>
     </row>
@@ -6649,7 +6651,7 @@
       </c>
       <c r="C52" s="61" t="str">
         <f>_xll.qlIMMNextCode(C51,B52,Trigger)</f>
-        <v>M9</v>
+        <v>U9</v>
       </c>
       <c r="D52" s="121"/>
       <c r="E52" s="121"/>
@@ -6660,11 +6662,11 @@
       </c>
       <c r="H52" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MM9_Quote</v>
+        <v>EURFUT3MU9_Quote</v>
       </c>
       <c r="I52" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MM9ConvAdj_Quote</v>
+        <v>EURFUT3MU9ConvAdj_Quote</v>
       </c>
       <c r="J52" s="62"/>
       <c r="L52" s="132" t="str">
@@ -6741,7 +6743,7 @@
       </c>
       <c r="C53" s="61" t="str">
         <f>_xll.qlIMMNextCode(C52,B53,Trigger)</f>
-        <v>U9</v>
+        <v>Z9</v>
       </c>
       <c r="D53" s="121"/>
       <c r="E53" s="121"/>
@@ -6752,11 +6754,11 @@
       </c>
       <c r="H53" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MU9_Quote</v>
+        <v>EURFUT3MZ9_Quote</v>
       </c>
       <c r="I53" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MU9ConvAdj_Quote</v>
+        <v>EURFUT3MZ9ConvAdj_Quote</v>
       </c>
       <c r="J53" s="62"/>
       <c r="L53" s="69" t="str">
@@ -6833,7 +6835,7 @@
       </c>
       <c r="C54" s="61" t="str">
         <f>_xll.qlIMMNextCode(C53,B54,Trigger)</f>
-        <v>Z9</v>
+        <v>H0</v>
       </c>
       <c r="D54" s="121"/>
       <c r="E54" s="121"/>
@@ -6844,11 +6846,11 @@
       </c>
       <c r="H54" s="115" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MZ9_Quote</v>
+        <v>EURFUT3MH0_Quote</v>
       </c>
       <c r="I54" s="115" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MZ9ConvAdj_Quote</v>
+        <v>EURFUT3MH0ConvAdj_Quote</v>
       </c>
       <c r="J54" s="62"/>
       <c r="L54" s="69" t="str">
@@ -6925,7 +6927,7 @@
       </c>
       <c r="C55" s="8" t="str">
         <f>_xll.qlIMMNextCode(C54,B55,Trigger)</f>
-        <v>H0</v>
+        <v>M0</v>
       </c>
       <c r="D55" s="122"/>
       <c r="E55" s="122"/>
@@ -6936,11 +6938,11 @@
       </c>
       <c r="H55" s="116" t="str">
         <f t="shared" si="15"/>
-        <v>EURFUT3MH0_Quote</v>
+        <v>EURFUT3MM0_Quote</v>
       </c>
       <c r="I55" s="116" t="str">
         <f t="shared" si="16"/>
-        <v>EURFUT3MH0ConvAdj_Quote</v>
+        <v>EURFUT3MM0ConvAdj_Quote</v>
       </c>
       <c r="J55" s="2"/>
       <c r="L55" s="69" t="str">
@@ -7021,7 +7023,7 @@
       </c>
       <c r="M56" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00563#0001</v>
+        <v>obj_00578#0000</v>
       </c>
       <c r="N56" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M56,Trigger),"--")</f>
@@ -7029,7 +7031,7 @@
       </c>
       <c r="O56" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M56,Trigger),"--")</f>
-        <v>5.6999999999999998E-4</v>
+        <v>-4.2999999999999999E-4</v>
       </c>
       <c r="P56" s="138" t="b">
         <v>1</v>
@@ -7042,11 +7044,11 @@
       </c>
       <c r="S56" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M56,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T56" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M56,Trigger),"--")</f>
-        <v>43003</v>
+        <v>43038</v>
       </c>
       <c r="V56" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7117,7 +7119,7 @@
       </c>
       <c r="M57" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00551#0001</v>
+        <v>obj_00562#0000</v>
       </c>
       <c r="N57" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M57,Trigger),"--")</f>
@@ -7125,7 +7127,7 @@
       </c>
       <c r="O57" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M57,Trigger),"--")</f>
-        <v>1.2800000000000001E-3</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="P57" s="138" t="b">
         <v>1</v>
@@ -7138,11 +7140,11 @@
       </c>
       <c r="S57" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M57,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T57" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M57,Trigger),"--")</f>
-        <v>43368</v>
+        <v>43402</v>
       </c>
       <c r="V57" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7213,7 +7215,7 @@
       </c>
       <c r="M58" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00552#0001</v>
+        <v>obj_00565#0000</v>
       </c>
       <c r="N58" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M58,Trigger),"--")</f>
@@ -7221,7 +7223,7 @@
       </c>
       <c r="O58" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M58,Trigger),"--")</f>
-        <v>2.3899999999999998E-3</v>
+        <v>1.1100000000000001E-3</v>
       </c>
       <c r="P58" s="138" t="b">
         <v>1</v>
@@ -7234,11 +7236,11 @@
       </c>
       <c r="S58" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M58,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T58" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M58,Trigger),"--")</f>
-        <v>43733</v>
+        <v>43767</v>
       </c>
       <c r="V58" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7309,7 +7311,7 @@
       </c>
       <c r="M59" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00558#0001</v>
+        <v>obj_0055e#0000</v>
       </c>
       <c r="N59" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M59,Trigger),"--")</f>
@@ -7317,7 +7319,7 @@
       </c>
       <c r="O59" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M59,Trigger),"--")</f>
-        <v>3.6800000000000001E-3</v>
+        <v>2.2699999999999999E-3</v>
       </c>
       <c r="P59" s="138" t="b">
         <v>1</v>
@@ -7330,11 +7332,11 @@
       </c>
       <c r="S59" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M59,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T59" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M59,Trigger),"--")</f>
-        <v>44099</v>
+        <v>44133</v>
       </c>
       <c r="V59" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7405,7 +7407,7 @@
       </c>
       <c r="M60" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00550#0001</v>
+        <v>obj_0055d#0000</v>
       </c>
       <c r="N60" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M60,Trigger),"--")</f>
@@ -7413,7 +7415,7 @@
       </c>
       <c r="O60" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M60,Trigger),"--")</f>
-        <v>5.0200000000000002E-3</v>
+        <v>3.5099999999999997E-3</v>
       </c>
       <c r="P60" s="138" t="b">
         <v>1</v>
@@ -7426,11 +7428,11 @@
       </c>
       <c r="S60" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M60,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T60" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M60,Trigger),"--")</f>
-        <v>44466</v>
+        <v>44498</v>
       </c>
       <c r="V60" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7501,7 +7503,7 @@
       </c>
       <c r="M61" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0056d#0001</v>
+        <v>obj_0055b#0000</v>
       </c>
       <c r="N61" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M61,Trigger),"--")</f>
@@ -7509,7 +7511,7 @@
       </c>
       <c r="O61" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M61,Trigger),"--")</f>
-        <v>6.3599999999999993E-3</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="P61" s="138" t="b">
         <v>1</v>
@@ -7522,11 +7524,11 @@
       </c>
       <c r="S61" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M61,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T61" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M61,Trigger),"--")</f>
-        <v>44830</v>
+        <v>44865</v>
       </c>
       <c r="V61" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7592,7 +7594,7 @@
       </c>
       <c r="J62" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H62,,B62,Calendar,D62,E62,F62,G62,I62,C62,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00563#0001</v>
+        <v>obj_00578#0000</v>
       </c>
       <c r="L62" s="69" t="str">
         <f t="shared" si="18"/>
@@ -7600,7 +7602,7 @@
       </c>
       <c r="M62" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0055d#0001</v>
+        <v>obj_00573#0000</v>
       </c>
       <c r="N62" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M62,Trigger),"--")</f>
@@ -7608,7 +7610,7 @@
       </c>
       <c r="O62" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M62,Trigger),"--")</f>
-        <v>7.6499999999999988E-3</v>
+        <v>6.0499999999999998E-3</v>
       </c>
       <c r="P62" s="138" t="b">
         <v>1</v>
@@ -7621,11 +7623,11 @@
       </c>
       <c r="S62" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M62,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T62" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M62,Trigger),"--")</f>
-        <v>45194</v>
+        <v>45229</v>
       </c>
       <c r="V62" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7691,7 +7693,7 @@
       </c>
       <c r="J63" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H63,,B63,Calendar,D63,E63,F63,G63,I63,C63,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00551#0001</v>
+        <v>obj_00562#0000</v>
       </c>
       <c r="L63" s="69" t="str">
         <f t="shared" si="18"/>
@@ -7699,7 +7701,7 @@
       </c>
       <c r="M63" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00567#0001</v>
+        <v>obj_00564#0000</v>
       </c>
       <c r="N63" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M63,Trigger),"--")</f>
@@ -7707,7 +7709,7 @@
       </c>
       <c r="O63" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M63,Trigger),"--")</f>
-        <v>8.8400000000000006E-3</v>
+        <v>7.2099999999999994E-3</v>
       </c>
       <c r="P63" s="138" t="b">
         <v>1</v>
@@ -7720,11 +7722,11 @@
       </c>
       <c r="S63" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M63,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T63" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M63,Trigger),"--")</f>
-        <v>45560</v>
+        <v>45594</v>
       </c>
       <c r="V63" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7790,7 +7792,7 @@
       </c>
       <c r="J64" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H64,,B64,Calendar,D64,E64,F64,G64,I64,C64,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00552#0001</v>
+        <v>obj_00565#0000</v>
       </c>
       <c r="L64" s="69" t="str">
         <f t="shared" si="18"/>
@@ -7798,7 +7800,7 @@
       </c>
       <c r="M64" s="137" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0055c#0001</v>
+        <v>obj_00561#0000</v>
       </c>
       <c r="N64" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M64,Trigger),"--")</f>
@@ -7806,7 +7808,7 @@
       </c>
       <c r="O64" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M64,Trigger),"--")</f>
-        <v>9.8999999999999991E-3</v>
+        <v>8.2700000000000013E-3</v>
       </c>
       <c r="P64" s="138" t="b">
         <v>1</v>
@@ -7819,11 +7821,11 @@
       </c>
       <c r="S64" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M64,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T64" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M64,Trigger),"--")</f>
-        <v>45925</v>
+        <v>45959</v>
       </c>
       <c r="V64" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7889,7 +7891,7 @@
       </c>
       <c r="J65" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H65,,B65,Calendar,D65,E65,F65,G65,I65,C65,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00558#0001</v>
+        <v>obj_0055e#0000</v>
       </c>
       <c r="L65" s="69" t="str">
         <f t="shared" si="18"/>
@@ -7897,7 +7899,7 @@
       </c>
       <c r="M65" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00559#0001</v>
+        <v>obj_00566#0000</v>
       </c>
       <c r="N65" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M65,Trigger),"--")</f>
@@ -7905,7 +7907,7 @@
       </c>
       <c r="O65" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M65,Trigger),"--")</f>
-        <v>1.0860000000000002E-2</v>
+        <v>9.2299999999999986E-3</v>
       </c>
       <c r="P65" s="138" t="b">
         <v>1</v>
@@ -7918,11 +7920,11 @@
       </c>
       <c r="S65" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M65,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T65" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M65,Trigger),"--")</f>
-        <v>46290</v>
+        <v>46324</v>
       </c>
       <c r="V65" s="3" t="str">
         <f t="shared" si="17"/>
@@ -7988,7 +7990,7 @@
       </c>
       <c r="J66" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H66,,B66,Calendar,D66,E66,F66,G66,I66,C66,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00550#0001</v>
+        <v>obj_0055d#0000</v>
       </c>
       <c r="L66" s="69" t="str">
         <f t="shared" si="18"/>
@@ -7996,7 +7998,7 @@
       </c>
       <c r="M66" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00560#0001</v>
+        <v>obj_00563#0000</v>
       </c>
       <c r="N66" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M66,Trigger),"--")</f>
@@ -8004,7 +8006,7 @@
       </c>
       <c r="O66" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M66,Trigger),"--")</f>
-        <v>1.171E-2</v>
+        <v>1.0089999999999998E-2</v>
       </c>
       <c r="P66" s="138" t="b">
         <v>1</v>
@@ -8017,11 +8019,11 @@
       </c>
       <c r="S66" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M66,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T66" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M66,Trigger),"--")</f>
-        <v>46657</v>
+        <v>46689</v>
       </c>
       <c r="V66" s="3" t="str">
         <f t="shared" si="17"/>
@@ -8087,7 +8089,7 @@
       </c>
       <c r="J67" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H67,,B67,Calendar,D67,E67,F67,G67,I67,C67,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0056d#0001</v>
+        <v>obj_0055b#0000</v>
       </c>
       <c r="L67" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8095,7 +8097,7 @@
       </c>
       <c r="M67" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00556#0001</v>
+        <v>obj_00572#0000</v>
       </c>
       <c r="N67" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M67,Trigger),"--")</f>
@@ -8103,7 +8105,7 @@
       </c>
       <c r="O67" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M67,Trigger),"--")</f>
-        <v>1.2450000000000001E-2</v>
+        <v>1.0840000000000001E-2</v>
       </c>
       <c r="P67" s="138" t="b">
         <v>1</v>
@@ -8116,11 +8118,11 @@
       </c>
       <c r="S67" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M67,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T67" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M67,Trigger),"--")</f>
-        <v>47021</v>
+        <v>47056</v>
       </c>
       <c r="V67" s="3" t="str">
         <f t="shared" ref="V67:V89" si="22">IFERROR(INDEX($L$3:$L$89,MATCH(X67,$N$3:$N$89,0),1),"")</f>
@@ -8186,7 +8188,7 @@
       </c>
       <c r="J68" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H68,,B68,Calendar,D68,E68,F68,G68,I68,C68,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0055d#0001</v>
+        <v>obj_00573#0000</v>
       </c>
       <c r="L68" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8194,7 +8196,7 @@
       </c>
       <c r="M68" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00561#0001</v>
+        <v>obj_0056c#0000</v>
       </c>
       <c r="N68" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M68,Trigger),"--")</f>
@@ -8202,7 +8204,7 @@
       </c>
       <c r="O68" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M68,Trigger),"--")</f>
-        <v>1.307E-2</v>
+        <v>1.1480000000000001E-2</v>
       </c>
       <c r="P68" s="138" t="b">
         <v>1</v>
@@ -8215,11 +8217,11 @@
       </c>
       <c r="S68" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M68,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T68" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M68,Trigger),"--")</f>
-        <v>47386</v>
+        <v>47420</v>
       </c>
       <c r="V68" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8285,7 +8287,7 @@
       </c>
       <c r="J69" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H69,,B69,Calendar,D69,E69,F69,G69,I69,C69,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00567#0001</v>
+        <v>obj_00564#0000</v>
       </c>
       <c r="L69" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8293,7 +8295,7 @@
       </c>
       <c r="M69" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00554#0001</v>
+        <v>obj_0056e#0000</v>
       </c>
       <c r="N69" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M69,Trigger),"--")</f>
@@ -8301,7 +8303,7 @@
       </c>
       <c r="O69" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M69,Trigger),"--")</f>
-        <v>1.359E-2</v>
+        <v>1.204E-2</v>
       </c>
       <c r="P69" s="138" t="b">
         <v>1</v>
@@ -8314,11 +8316,11 @@
       </c>
       <c r="S69" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M69,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T69" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M69,Trigger),"--")</f>
-        <v>47751</v>
+        <v>47785</v>
       </c>
       <c r="V69" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8384,7 +8386,7 @@
       </c>
       <c r="J70" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H70,,B70,Calendar,D70,E70,F70,G70,I70,C70,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0055c#0001</v>
+        <v>obj_00561#0000</v>
       </c>
       <c r="L70" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8392,7 +8394,7 @@
       </c>
       <c r="M70" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00570#0001</v>
+        <v>obj_0056d#0000</v>
       </c>
       <c r="N70" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M70,Trigger),"--")</f>
@@ -8400,7 +8402,7 @@
       </c>
       <c r="O70" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M70,Trigger),"--")</f>
-        <v>1.4030000000000001E-2</v>
+        <v>1.252E-2</v>
       </c>
       <c r="P70" s="138" t="b">
         <v>1</v>
@@ -8413,11 +8415,11 @@
       </c>
       <c r="S70" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M70,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T70" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M70,Trigger),"--")</f>
-        <v>48116</v>
+        <v>48150</v>
       </c>
       <c r="V70" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8483,7 +8485,7 @@
       </c>
       <c r="J71" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H71,,B71,Calendar,D71,E71,F71,G71,I71,C71,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00559#0001</v>
+        <v>obj_00566#0000</v>
       </c>
       <c r="L71" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8491,7 +8493,7 @@
       </c>
       <c r="M71" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00564#0001</v>
+        <v>obj_00574#0000</v>
       </c>
       <c r="N71" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M71,Trigger),"--")</f>
@@ -8499,7 +8501,7 @@
       </c>
       <c r="O71" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M71,Trigger),"--")</f>
-        <v>1.44E-2</v>
+        <v>1.2920000000000001E-2</v>
       </c>
       <c r="P71" s="138" t="b">
         <v>1</v>
@@ -8512,11 +8514,11 @@
       </c>
       <c r="S71" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M71,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T71" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M71,Trigger),"--")</f>
-        <v>48484</v>
+        <v>48516</v>
       </c>
       <c r="V71" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8582,7 +8584,7 @@
       </c>
       <c r="J72" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H72,,B72,Calendar,D72,E72,F72,G72,I72,C72,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00560#0001</v>
+        <v>obj_00563#0000</v>
       </c>
       <c r="L72" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8590,7 +8592,7 @@
       </c>
       <c r="M72" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0055a#0001</v>
+        <v>obj_0056b#0000</v>
       </c>
       <c r="N72" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M72,Trigger),"--")</f>
@@ -8598,7 +8600,7 @@
       </c>
       <c r="O72" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M72,Trigger),"--")</f>
-        <v>1.47E-2</v>
+        <v>1.3260000000000001E-2</v>
       </c>
       <c r="P72" s="138" t="b">
         <v>1</v>
@@ -8611,11 +8613,11 @@
       </c>
       <c r="S72" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M72,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T72" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M72,Trigger),"--")</f>
-        <v>48848</v>
+        <v>48883</v>
       </c>
       <c r="V72" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8681,7 +8683,7 @@
       </c>
       <c r="J73" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H73,,B73,Calendar,D73,E73,F73,G73,I73,C73,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00556#0001</v>
+        <v>obj_00572#0000</v>
       </c>
       <c r="L73" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8689,7 +8691,7 @@
       </c>
       <c r="M73" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00557#0001</v>
+        <v>obj_00557#0000</v>
       </c>
       <c r="N73" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M73,Trigger),"--")</f>
@@ -8697,7 +8699,7 @@
       </c>
       <c r="O73" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M73,Trigger),"--")</f>
-        <v>1.4929999999999999E-2</v>
+        <v>1.3540000000000002E-2</v>
       </c>
       <c r="P73" s="138" t="b">
         <v>1</v>
@@ -8710,11 +8712,11 @@
       </c>
       <c r="S73" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M73,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T73" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M73,Trigger),"--")</f>
-        <v>49212</v>
+        <v>49247</v>
       </c>
       <c r="V73" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8780,7 +8782,7 @@
       </c>
       <c r="J74" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H74,,B74,Calendar,D74,E74,F74,G74,I74,C74,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00561#0001</v>
+        <v>obj_0056c#0000</v>
       </c>
       <c r="L74" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8788,7 +8790,7 @@
       </c>
       <c r="M74" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0056e#0001</v>
+        <v>obj_00576#0000</v>
       </c>
       <c r="N74" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M74,Trigger),"--")</f>
@@ -8796,7 +8798,7 @@
       </c>
       <c r="O74" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M74,Trigger),"--")</f>
-        <v>1.5110000000000002E-2</v>
+        <v>1.375E-2</v>
       </c>
       <c r="P74" s="138" t="b">
         <v>1</v>
@@ -8809,11 +8811,11 @@
       </c>
       <c r="S74" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M74,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T74" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M74,Trigger),"--")</f>
-        <v>49577</v>
+        <v>49611</v>
       </c>
       <c r="V74" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8879,7 +8881,7 @@
       </c>
       <c r="J75" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H75,,B75,Calendar,D75,E75,F75,G75,I75,C75,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00554#0001</v>
+        <v>obj_0056e#0000</v>
       </c>
       <c r="L75" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8887,7 +8889,7 @@
       </c>
       <c r="M75" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0055f#0001</v>
+        <v>obj_0055f#0000</v>
       </c>
       <c r="N75" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M75,Trigger),"--")</f>
@@ -8895,7 +8897,7 @@
       </c>
       <c r="O75" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M75,Trigger),"--")</f>
-        <v>1.525E-2</v>
+        <v>1.3919999999999998E-2</v>
       </c>
       <c r="P75" s="138" t="b">
         <v>1</v>
@@ -8908,11 +8910,11 @@
       </c>
       <c r="S75" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M75,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T75" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M75,Trigger),"--")</f>
-        <v>49943</v>
+        <v>49977</v>
       </c>
       <c r="V75" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8978,7 +8980,7 @@
       </c>
       <c r="J76" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H76,,B76,Calendar,D76,E76,F76,G76,I76,C76,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00570#0001</v>
+        <v>obj_0056d#0000</v>
       </c>
       <c r="L76" s="69" t="str">
         <f t="shared" si="18"/>
@@ -8986,7 +8988,7 @@
       </c>
       <c r="M76" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0056b#0001</v>
+        <v>obj_0055c#0000</v>
       </c>
       <c r="N76" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M76,Trigger),"--")</f>
@@ -8994,7 +8996,7 @@
       </c>
       <c r="O76" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M76,Trigger),"--")</f>
-        <v>1.5339999999999999E-2</v>
+        <v>1.4039999999999999E-2</v>
       </c>
       <c r="P76" s="138" t="b">
         <v>1</v>
@@ -9007,11 +9009,11 @@
       </c>
       <c r="S76" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M76,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T76" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M76,Trigger),"--")</f>
-        <v>50308</v>
+        <v>50342</v>
       </c>
       <c r="V76" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9077,7 +9079,7 @@
       </c>
       <c r="J77" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H77,,B77,Calendar,D77,E77,F77,G77,I77,C77,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00564#0001</v>
+        <v>obj_00574#0000</v>
       </c>
       <c r="L77" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9085,7 +9087,7 @@
       </c>
       <c r="M77" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0056c#0001</v>
+        <v>obj_00575#0000</v>
       </c>
       <c r="N77" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M77,Trigger),"--")</f>
@@ -9093,7 +9095,7 @@
       </c>
       <c r="O77" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M77,Trigger),"--")</f>
-        <v>1.541E-2</v>
+        <v>1.4119999999999999E-2</v>
       </c>
       <c r="P77" s="138" t="b">
         <v>1</v>
@@ -9106,11 +9108,11 @@
       </c>
       <c r="S77" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M77,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T77" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M77,Trigger),"--")</f>
-        <v>50675</v>
+        <v>50707</v>
       </c>
       <c r="V77" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9176,7 +9178,7 @@
       </c>
       <c r="J78" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H78,,B78,Calendar,D78,E78,F78,G78,I78,C78,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0055a#0001</v>
+        <v>obj_0056b#0000</v>
       </c>
       <c r="L78" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9184,7 +9186,7 @@
       </c>
       <c r="M78" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00571#0001</v>
+        <v>obj_00577#0000</v>
       </c>
       <c r="N78" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M78,Trigger),"--")</f>
@@ -9192,7 +9194,7 @@
       </c>
       <c r="O78" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M78,Trigger),"--")</f>
-        <v>1.5449999999999998E-2</v>
+        <v>1.4180000000000002E-2</v>
       </c>
       <c r="P78" s="138" t="b">
         <v>1</v>
@@ -9205,11 +9207,11 @@
       </c>
       <c r="S78" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M78,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T78" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M78,Trigger),"--")</f>
-        <v>51039</v>
+        <v>51074</v>
       </c>
       <c r="V78" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9275,7 +9277,7 @@
       </c>
       <c r="J79" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H79,,B79,Calendar,D79,E79,F79,G79,I79,C79,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00557#0001</v>
+        <v>obj_00557#0000</v>
       </c>
       <c r="L79" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9283,7 +9285,7 @@
       </c>
       <c r="M79" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0056a#0001</v>
+        <v>obj_00571#0000</v>
       </c>
       <c r="N79" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M79,Trigger),"--")</f>
@@ -9291,7 +9293,7 @@
       </c>
       <c r="O79" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M79,Trigger),"--")</f>
-        <v>1.5480000000000001E-2</v>
+        <v>1.423E-2</v>
       </c>
       <c r="P79" s="138" t="b">
         <v>1</v>
@@ -9304,11 +9306,11 @@
       </c>
       <c r="S79" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M79,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T79" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M79,Trigger),"--")</f>
-        <v>51404</v>
+        <v>51438</v>
       </c>
       <c r="V79" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9374,7 +9376,7 @@
       </c>
       <c r="J80" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H80,,B80,Calendar,D80,E80,F80,G80,I80,C80,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0056e#0001</v>
+        <v>obj_00576#0000</v>
       </c>
       <c r="L80" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9382,7 +9384,7 @@
       </c>
       <c r="M80" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00553#0001</v>
+        <v>obj_0056a#0000</v>
       </c>
       <c r="N80" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M80,Trigger),"--")</f>
@@ -9390,7 +9392,7 @@
       </c>
       <c r="O80" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M80,Trigger),"--")</f>
-        <v>1.55E-2</v>
+        <v>1.427E-2</v>
       </c>
       <c r="P80" s="138" t="b">
         <v>1</v>
@@ -9403,11 +9405,11 @@
       </c>
       <c r="S80" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M80,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T80" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M80,Trigger),"--")</f>
-        <v>51769</v>
+        <v>51803</v>
       </c>
       <c r="V80" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9473,7 +9475,7 @@
       </c>
       <c r="J81" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H81,,B81,Calendar,D81,E81,F81,G81,I81,C81,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0055f#0001</v>
+        <v>obj_0055f#0000</v>
       </c>
       <c r="L81" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9481,7 +9483,7 @@
       </c>
       <c r="M81" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00569#0001</v>
+        <v>obj_00560#0000</v>
       </c>
       <c r="N81" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M81,Trigger),"--")</f>
@@ -9489,7 +9491,7 @@
       </c>
       <c r="O81" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M81,Trigger),"--")</f>
-        <v>1.5509999999999999E-2</v>
+        <v>1.43E-2</v>
       </c>
       <c r="P81" s="138" t="b">
         <v>1</v>
@@ -9502,11 +9504,11 @@
       </c>
       <c r="S81" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M81,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T81" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M81,Trigger),"--")</f>
-        <v>52134</v>
+        <v>52168</v>
       </c>
       <c r="V81" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9572,7 +9574,7 @@
       </c>
       <c r="J82" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H82,,B82,Calendar,D82,E82,F82,G82,I82,C82,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0056b#0001</v>
+        <v>obj_0055c#0000</v>
       </c>
       <c r="L82" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9580,7 +9582,7 @@
       </c>
       <c r="M82" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00565#0001</v>
+        <v>obj_00559#0000</v>
       </c>
       <c r="N82" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M82,Trigger),"--")</f>
@@ -9588,7 +9590,7 @@
       </c>
       <c r="O82" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M82,Trigger),"--")</f>
-        <v>1.5520000000000001E-2</v>
+        <v>1.4339999999999999E-2</v>
       </c>
       <c r="P82" s="138" t="b">
         <v>1</v>
@@ -9601,11 +9603,11 @@
       </c>
       <c r="S82" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M82,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T82" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M82,Trigger),"--")</f>
-        <v>52499</v>
+        <v>52533</v>
       </c>
       <c r="V82" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9671,7 +9673,7 @@
       </c>
       <c r="J83" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H83,,B83,Calendar,D83,E83,F83,G83,I83,C83,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0056c#0001</v>
+        <v>obj_00575#0000</v>
       </c>
       <c r="L83" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9679,7 +9681,7 @@
       </c>
       <c r="M83" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00555#0001</v>
+        <v>obj_00569#0000</v>
       </c>
       <c r="N83" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M83,Trigger),"--")</f>
@@ -9687,7 +9689,7 @@
       </c>
       <c r="O83" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M83,Trigger),"--")</f>
-        <v>1.5529999999999999E-2</v>
+        <v>1.4370000000000001E-2</v>
       </c>
       <c r="P83" s="138" t="b">
         <v>1</v>
@@ -9700,11 +9702,11 @@
       </c>
       <c r="S83" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M83,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T83" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M83,Trigger),"--")</f>
-        <v>52866</v>
+        <v>52901</v>
       </c>
       <c r="V83" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9770,7 +9772,7 @@
       </c>
       <c r="J84" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H84,,B84,Calendar,D84,E84,F84,G84,I84,C84,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00571#0001</v>
+        <v>obj_00577#0000</v>
       </c>
       <c r="L84" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9778,7 +9780,7 @@
       </c>
       <c r="M84" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00568#0001</v>
+        <v>obj_00567#0000</v>
       </c>
       <c r="N84" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M84,Trigger),"--")</f>
@@ -9786,7 +9788,7 @@
       </c>
       <c r="O84" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M84,Trigger),"--")</f>
-        <v>1.554E-2</v>
+        <v>1.439E-2</v>
       </c>
       <c r="P84" s="138" t="b">
         <v>1</v>
@@ -9799,11 +9801,11 @@
       </c>
       <c r="S84" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M84,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T84" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M84,Trigger),"--")</f>
-        <v>53230</v>
+        <v>53265</v>
       </c>
       <c r="V84" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9869,7 +9871,7 @@
       </c>
       <c r="J85" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H85,,B85,Calendar,D85,E85,F85,G85,I85,C85,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0056a#0001</v>
+        <v>obj_00571#0000</v>
       </c>
       <c r="L85" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9877,7 +9879,7 @@
       </c>
       <c r="M85" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_00562#0001</v>
+        <v>obj_00570#0000</v>
       </c>
       <c r="N85" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M85,Trigger),"--")</f>
@@ -9885,7 +9887,7 @@
       </c>
       <c r="O85" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M85,Trigger),"--")</f>
-        <v>1.5600000000000001E-2</v>
+        <v>1.4490000000000001E-2</v>
       </c>
       <c r="P85" s="138" t="b">
         <v>1</v>
@@ -9898,11 +9900,11 @@
       </c>
       <c r="S85" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M85,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T85" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M85,Trigger),"--")</f>
-        <v>55057</v>
+        <v>55092</v>
       </c>
       <c r="V85" s="3" t="str">
         <f t="shared" si="22"/>
@@ -9968,7 +9970,7 @@
       </c>
       <c r="J86" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H86,,B86,Calendar,D86,E86,F86,G86,I86,C86,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00553#0001</v>
+        <v>obj_0056a#0000</v>
       </c>
       <c r="L86" s="69" t="str">
         <f t="shared" si="18"/>
@@ -9976,7 +9978,7 @@
       </c>
       <c r="M86" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0055e#0001</v>
+        <v>obj_00558#0000</v>
       </c>
       <c r="N86" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M86,Trigger),"--")</f>
@@ -9984,7 +9986,7 @@
       </c>
       <c r="O86" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M86,Trigger),"--")</f>
-        <v>1.5600000000000001E-2</v>
+        <v>1.4499999999999999E-2</v>
       </c>
       <c r="P86" s="138" t="b">
         <v>1</v>
@@ -9997,11 +9999,11 @@
       </c>
       <c r="S86" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M86,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T86" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M86,Trigger),"--")</f>
-        <v>56884</v>
+        <v>56916</v>
       </c>
       <c r="V86" s="3" t="str">
         <f t="shared" si="22"/>
@@ -10067,7 +10069,7 @@
       </c>
       <c r="J87" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H87,,B87,Calendar,D87,E87,F87,G87,I87,C87,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00569#0001</v>
+        <v>obj_00560#0000</v>
       </c>
       <c r="L87" s="69" t="str">
         <f t="shared" si="18"/>
@@ -10166,7 +10168,7 @@
       </c>
       <c r="J88" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H88,,B88,Calendar,D88,E88,F88,G88,I88,C88,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00565#0001</v>
+        <v>obj_00559#0000</v>
       </c>
       <c r="K88" s="47" t="s">
         <v>36</v>
@@ -10177,7 +10179,7 @@
       </c>
       <c r="M88" s="138" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0055b#0001</v>
+        <v>obj_0056f#0000</v>
       </c>
       <c r="N88" s="146" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M88,Trigger),"--")</f>
@@ -10185,7 +10187,7 @@
       </c>
       <c r="O88" s="139">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M88,Trigger),"--")</f>
-        <v>1.5169999999999999E-2</v>
+        <v>1.4079999999999999E-2</v>
       </c>
       <c r="P88" s="138" t="b">
         <v>1</v>
@@ -10198,11 +10200,11 @@
       </c>
       <c r="S88" s="140">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M88,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T88" s="140">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M88,Trigger),"--")</f>
-        <v>60535</v>
+        <v>60569</v>
       </c>
       <c r="V88" s="3" t="str">
         <f t="shared" si="22"/>
@@ -10268,7 +10270,7 @@
       </c>
       <c r="J89" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H89,,B89,Calendar,D89,E89,F89,G89,I89,C89,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00555#0001</v>
+        <v>obj_00569#0000</v>
       </c>
       <c r="L89" s="70" t="str">
         <f t="shared" si="18"/>
@@ -10276,7 +10278,7 @@
       </c>
       <c r="M89" s="141" t="str">
         <f t="shared" si="19"/>
-        <v>obj_0056f#0001</v>
+        <v>obj_00568#0000</v>
       </c>
       <c r="N89" s="151" t="str">
         <f>IFERROR(_xll.qlRateHelperQuoteName(M89,Trigger),"--")</f>
@@ -10284,7 +10286,7 @@
       </c>
       <c r="O89" s="152">
         <f>IFERROR(_xll.qlRateHelperQuoteValue($M89,Trigger),"--")</f>
-        <v>1.502E-2</v>
+        <v>1.393E-2</v>
       </c>
       <c r="P89" s="141" t="b">
         <v>1</v>
@@ -10297,11 +10299,11 @@
       </c>
       <c r="S89" s="150">
         <f>IFERROR(_xll.qlRateHelperEarliestDate(M89,Trigger),"--")</f>
-        <v>42272</v>
+        <v>42306</v>
       </c>
       <c r="T89" s="150">
         <f>IFERROR(_xll.qlRateHelperPillarDate(M89,Trigger),"--")</f>
-        <v>64187</v>
+        <v>64221</v>
       </c>
       <c r="V89" s="5" t="str">
         <f t="shared" si="22"/>
@@ -10367,7 +10369,7 @@
       </c>
       <c r="J90" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H90,,B90,Calendar,D90,E90,F90,G90,I90,C90,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00568#0001</v>
+        <v>obj_00567#0000</v>
       </c>
       <c r="AD90" s="158"/>
     </row>
@@ -10403,7 +10405,7 @@
       </c>
       <c r="J91" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H91,,B91,Calendar,D91,E91,F91,G91,I91,C91,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_00562#0001</v>
+        <v>obj_00570#0000</v>
       </c>
       <c r="AD91" s="158"/>
     </row>
@@ -10439,7 +10441,7 @@
       </c>
       <c r="J92" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H92,,B92,Calendar,D92,E92,F92,G92,I92,C92,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0055e#0001</v>
+        <v>obj_00558#0000</v>
       </c>
       <c r="AD92" s="158"/>
     </row>
@@ -10508,7 +10510,7 @@
       </c>
       <c r="J94" s="62" t="str">
         <f>_xll.qlSwapRateHelper2(,H94,,B94,Calendar,D94,E94,F94,G94,I94,C94,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0055b#0001</v>
+        <v>obj_0056f#0000</v>
       </c>
       <c r="AD94" s="158"/>
     </row>
@@ -10544,7 +10546,7 @@
       </c>
       <c r="J95" s="2" t="str">
         <f>_xll.qlSwapRateHelper2(,H95,,B95,Calendar,D95,E95,F95,G95,I95,C95,Discounting,PillarDate,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>obj_0056f#0001</v>
+        <v>obj_00568#0000</v>
       </c>
       <c r="AD95" s="158"/>
     </row>

</xml_diff>